<commit_message>
Save FPTS projections to file
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Player</t>
   </si>
@@ -54,49 +54,46 @@
     <t>???</t>
   </si>
   <si>
-    <t>Los Angeles Dodgers righties</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Verdugo</t>
-  </si>
-  <si>
-    <t>Kemp</t>
-  </si>
-  <si>
-    <t>Pederson</t>
-  </si>
-  <si>
-    <t>Minnesota Twins hitters</t>
-  </si>
-  <si>
     <t>Mauer</t>
   </si>
   <si>
-    <t>Dozier</t>
-  </si>
-  <si>
-    <t>Garver</t>
-  </si>
-  <si>
-    <t>Morrison</t>
-  </si>
-  <si>
-    <t>Colorado Rockies righties</t>
-  </si>
-  <si>
-    <t>Desmond</t>
-  </si>
-  <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Iannetta</t>
-  </si>
-  <si>
-    <t>Cuevas</t>
+    <t>Toronto Blue Jays lefties</t>
+  </si>
+  <si>
+    <t>Solarte</t>
+  </si>
+  <si>
+    <t>Smoak</t>
+  </si>
+  <si>
+    <t>Morales</t>
+  </si>
+  <si>
+    <t>Tampa Bay Rays righties</t>
+  </si>
+  <si>
+    <t>Span</t>
+  </si>
+  <si>
+    <t>Cron</t>
+  </si>
+  <si>
+    <t>Duffy</t>
+  </si>
+  <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>Minnesota Twins lefties</t>
+  </si>
+  <si>
+    <t>Kepler</t>
+  </si>
+  <si>
+    <t>Rosario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morrison </t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:I9"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +496,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -557,166 +554,158 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5">
-        <v>3300</v>
+        <v>3800</v>
       </c>
       <c r="C3">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>5.7575757575757578</v>
+        <v>1.5789473684210527</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="5">
-        <v>3200</v>
+        <v>3000</v>
       </c>
       <c r="H3">
-        <v>18.399999999999999</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>5.75</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="L3" s="5">
-        <v>2700</v>
+        <v>3200</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>0</v>
+        <v>1.9375</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>0</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="5">
-        <v>3300</v>
+        <v>2900</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>0.90909090909090906</v>
+        <v>2.0689655172413794</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" s="5">
-        <v>3600</v>
+        <v>3300</v>
       </c>
       <c r="M4">
-        <v>9</v>
+        <v>3.5</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>2.5</v>
+        <v>1.0606060606060608</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5">
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="C5">
-        <v>28.2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>10.071428571428571</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="5">
-        <v>2100</v>
+        <v>2800</v>
       </c>
       <c r="H5">
-        <v>9.5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>4.5238095238095237</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L5" s="5">
-        <v>2300</v>
+        <v>3800</v>
       </c>
       <c r="M5">
-        <v>9.1999999999999993</v>
+        <v>34.4</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>9.0526315789473681</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2200</v>
-      </c>
-      <c r="C6">
-        <v>12.2</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="5"/>
+      <c r="D6" s="7" t="e">
         <f t="shared" si="0"/>
-        <v>5.545454545454545</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="5">
-        <v>2600</v>
+        <v>2700</v>
       </c>
       <c r="H6">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>2.3846153846153846</v>
+        <v>2.2222222222222223</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L6" s="5">
-        <v>2200</v>
+        <v>3000</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>1.3636363636363638</v>
+        <v>4.333333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -725,56 +714,56 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>10800</v>
+        <v>9900</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>59.400000000000006</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>5.5000000000000009</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>11200</v>
+        <v>11400</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>37.1</v>
+        <v>18</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>3.3125000000000004</v>
+        <v>1.5789473684210527</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>10800</v>
+        <v>13300</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>21.2</v>
+        <v>57.099999999999994</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>1.9629629629629628</v>
+        <v>4.2932330827067666</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -908,7 +897,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3">
         <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>3.5884146341463414</v>
+        <v>2.4306358381502888</v>
       </c>
     </row>
   </sheetData>
@@ -941,19 +930,19 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Los Angeles Dodgers righties|Taylor, Verdugo, Kemp, Pederson|$10,800|59.4|5.5x|Success|</v>
+        <v>|Toronto Blue Jays lefties|Solarte, Smoak, Morales, |$9,900|9|0.91x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Minnesota Twins hitters|Mauer, Dozier, Garver, Morrison|$11,200|37.1|3.31x|Failure|</v>
+        <v>|Tampa Bay Rays righties|Span, Cron, Duffy, Ramos|$11,400|18|1.58x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Colorado Rockies righties|Desmond, Story, Iannetta, Cuevas|$10,800|21.2|1.96x|Failure|</v>
+        <v>|Minnesota Twins lefties|Mauer, Kepler, Rosario, Morrison |$13,300|57.1|4.29x|Success|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Optimization of projections variables
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Player</t>
   </si>
@@ -54,46 +54,49 @@
     <t>???</t>
   </si>
   <si>
-    <t>Mauer</t>
-  </si>
-  <si>
-    <t>Toronto Blue Jays lefties</t>
-  </si>
-  <si>
-    <t>Solarte</t>
-  </si>
-  <si>
-    <t>Smoak</t>
-  </si>
-  <si>
-    <t>Morales</t>
-  </si>
-  <si>
-    <t>Tampa Bay Rays righties</t>
-  </si>
-  <si>
-    <t>Span</t>
-  </si>
-  <si>
-    <t>Cron</t>
-  </si>
-  <si>
-    <t>Duffy</t>
-  </si>
-  <si>
-    <t>Ramos</t>
-  </si>
-  <si>
-    <t>Minnesota Twins lefties</t>
-  </si>
-  <si>
-    <t>Kepler</t>
-  </si>
-  <si>
-    <t>Rosario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morrison </t>
+    <t>New York Mets hitters</t>
+  </si>
+  <si>
+    <t>Conforto</t>
+  </si>
+  <si>
+    <t>Cespedes</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>Detroit Tigers hitters</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Hicks</t>
+  </si>
+  <si>
+    <t>McCann</t>
+  </si>
+  <si>
+    <t>San Francisco Giants lefties</t>
+  </si>
+  <si>
+    <t>Blanco</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Crawford</t>
+  </si>
+  <si>
+    <t>Hanson</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +499,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -554,17 +557,17 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5">
-        <v>3800</v>
+        <v>3100</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>21.7</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>1.5789473684210527</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -573,139 +576,147 @@
         <v>3000</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>0</v>
+        <v>11.466666666666667</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="L3" s="5">
-        <v>3200</v>
+        <v>2400</v>
       </c>
       <c r="M3">
-        <v>6.2</v>
+        <v>3</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>1.9375</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>18.7</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>0.8571428571428571</v>
+        <v>4.6749999999999998</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="5">
-        <v>2900</v>
+        <v>2600</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>2.0689655172413794</v>
+        <v>3.8461538461538463</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L4" s="5">
-        <v>3300</v>
+        <v>3800</v>
       </c>
       <c r="M4">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>1.0606060606060608</v>
+        <v>0.78947368421052633</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5">
-        <v>2600</v>
+        <v>3100</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>31.2</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.064516129032258</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="5">
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>2.1428571428571428</v>
+        <v>1.153846153846154</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L5" s="5">
-        <v>3800</v>
+        <v>2800</v>
       </c>
       <c r="M5">
-        <v>34.4</v>
+        <v>3</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>9.0526315789473681</v>
+        <v>1.0714285714285714</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="D6" s="7" t="e">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>43.6</v>
+      </c>
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>17.440000000000001</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="5">
-        <v>2700</v>
+        <v>2400</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>2.2222222222222223</v>
+        <v>1.25</v>
       </c>
       <c r="K6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L6" s="5">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="M6">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>4.333333333333333</v>
+        <v>1.935483870967742</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -714,56 +725,56 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>9900</v>
+        <v>12700</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>9</v>
+        <v>115.19999999999999</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>0.90909090909090906</v>
+        <v>9.0708661417322833</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>11400</v>
+        <v>10600</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>18</v>
+        <v>50.4</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>1.5789473684210527</v>
+        <v>4.7547169811320753</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>13300</v>
+        <v>12100</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>57.099999999999994</v>
+        <v>15</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>4.2932330827067666</v>
+        <v>1.2396694214876034</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -897,7 +908,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3">
         <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>2.4306358381502888</v>
+        <v>5.101694915254237</v>
       </c>
     </row>
   </sheetData>
@@ -930,19 +941,19 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Toronto Blue Jays lefties|Solarte, Smoak, Morales, |$9,900|9|0.91x|Failure|</v>
+        <v>|New York Mets hitters|Conforto, Cespedes, Bruce, Gonzalez|$12,700|115.2|9.07x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Tampa Bay Rays righties|Span, Cron, Duffy, Ramos|$11,400|18|1.58x|Failure|</v>
+        <v>|Detroit Tigers hitters|Martin, Martinez, Hicks, McCann|$10,600|50.4|4.75x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Minnesota Twins lefties|Mauer, Kepler, Rosario, Morrison |$13,300|57.1|4.29x|Success|</v>
+        <v>|San Francisco Giants lefties|Blanco, Belt, Crawford, Hanson|$12,100|15|1.24x|Failure|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed insignificant Draftbook bug for pitcher/hitter AP weighting
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Player</t>
   </si>
@@ -48,52 +48,55 @@
     <t>???</t>
   </si>
   <si>
-    <t>Cincinnati Reds hitters</t>
-  </si>
-  <si>
-    <t>Peraza</t>
-  </si>
-  <si>
-    <t>Schebler</t>
-  </si>
-  <si>
-    <t>Suarez</t>
-  </si>
-  <si>
-    <t>Gennett</t>
-  </si>
-  <si>
-    <t>Baltimore Orioles righties</t>
-  </si>
-  <si>
-    <t>Mancini</t>
-  </si>
-  <si>
-    <t>Schoop</t>
-  </si>
-  <si>
-    <t>Trumbo</t>
-  </si>
-  <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>Philadelphia Phillies righties</t>
-  </si>
-  <si>
-    <t>Hernandez</t>
-  </si>
-  <si>
-    <t>Hoskins</t>
-  </si>
-  <si>
-    <t>Altherr</t>
-  </si>
-  <si>
-    <t>Santana</t>
-  </si>
-  <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Pham</t>
+  </si>
+  <si>
+    <t>Los Angeles Dodgers lefties</t>
+  </si>
+  <si>
+    <t>Pederson</t>
+  </si>
+  <si>
+    <t>Grandal</t>
+  </si>
+  <si>
+    <t>Bellinger</t>
+  </si>
+  <si>
+    <t>Puig</t>
+  </si>
+  <si>
+    <t>St. Louis Cardinals righties</t>
+  </si>
+  <si>
+    <t>Bader</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Ozuna</t>
+  </si>
+  <si>
+    <t>New York Yankees hitters</t>
+  </si>
+  <si>
+    <t>Gardner</t>
+  </si>
+  <si>
+    <t>Hicks</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Andujar</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,19 +499,19 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="F1" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
@@ -554,166 +557,167 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5">
-        <v>3300</v>
+        <v>2400</v>
       </c>
       <c r="C3">
-        <v>6.2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>1.8787878787878789</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G3" s="5">
-        <v>2900</v>
+        <v>3700</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>28.2</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>1.0344827586206897</v>
+        <v>7.6216216216216219</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L3" s="5">
-        <v>3400</v>
+        <v>3200</v>
       </c>
       <c r="M3">
-        <v>9.1999999999999993</v>
+        <v>15.2</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>2.7058823529411766</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="5">
-        <v>3000</v>
+        <v>3100</v>
       </c>
       <c r="C4">
-        <v>15.4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>5.1333333333333337</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" s="5">
-        <v>2600</v>
+        <v>2800</v>
       </c>
       <c r="H4">
-        <v>13.2</v>
+        <v>18.7</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>5.0769230769230766</v>
+        <v>6.6785714285714288</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L4" s="5">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5">
-        <v>3900</v>
+        <v>3400</v>
       </c>
       <c r="C5">
-        <v>32.4</v>
+        <v>9</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>8.3076923076923084</v>
+        <v>2.6470588235294117</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5" s="5">
-        <v>2700</v>
+        <v>3400</v>
       </c>
       <c r="H5">
-        <v>9.1999999999999993</v>
+        <v>3</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>3.407407407407407</v>
+        <v>0.88235294117647067</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L5" s="5">
-        <v>2400</v>
+        <v>2600</v>
       </c>
       <c r="M5">
-        <v>21.7</v>
+        <v>3</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>9.0416666666666661</v>
+        <v>1.153846153846154</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5">
-        <v>2800</v>
+        <v>2700</v>
       </c>
       <c r="C6">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>7.9285714285714288</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G6" s="5">
-        <v>2300</v>
+        <v>2800</v>
       </c>
       <c r="H6">
-        <v>28.2</v>
+        <f>18.7+6.2+6.2</f>
+        <v>31.099999999999998</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>12.260869565217391</v>
+        <v>11.107142857142858</v>
       </c>
       <c r="K6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L6" s="5">
-        <v>2600</v>
+        <v>2700</v>
       </c>
       <c r="M6">
-        <v>18.7</v>
+        <v>9.4</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>7.1923076923076925</v>
+        <v>3.4814814814814818</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -722,56 +726,56 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>13000</v>
+        <v>11600</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>76.2</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>5.8615384615384611</v>
+        <v>0.77586206896551724</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>10500</v>
+        <v>12700</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>53.599999999999994</v>
+        <v>81</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>5.1047619047619044</v>
+        <v>6.377952755905512</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>12400</v>
+        <v>11500</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>52.599999999999994</v>
+        <v>27.6</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>4.2419354838709671</v>
+        <v>2.4000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -905,7 +909,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3">
         <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>5.0807799442896941</v>
+        <v>3.2849162011173183</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +931,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,19 +942,19 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Cincinnati Reds hitters|Peraza, Schebler, Suarez, Gennett|$13,000|76.2|5.86x|Success|</v>
+        <v>|Los Angeles Dodgers lefties|Pederson, Grandal, Bellinger, Puig|$11,600|9|0.78x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Baltimore Orioles righties|Mancini, Schoop, Trumbo, Valencia|$10,500|53.6|5.1x|Success|</v>
+        <v>|St. Louis Cardinals righties|Pham, Bader, Martinez, Ozuna|$12,700|81|6.38x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Philadelphia Phillies righties|Hernandez, Hoskins, Altherr, Santana|$12,400|52.6|4.24x|Success|</v>
+        <v>|New York Yankees hitters|Gardner, Hicks, Walker, Andujar|$11,500|27.6|2.4x|Failure|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved overweighting of recent stats
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Player</t>
   </si>
@@ -48,55 +48,52 @@
     <t>???</t>
   </si>
   <si>
-    <t>Success</t>
-  </si>
-  <si>
     <t>Failure</t>
   </si>
   <si>
-    <t>Pham</t>
-  </si>
-  <si>
-    <t>Los Angeles Dodgers lefties</t>
-  </si>
-  <si>
     <t>Pederson</t>
   </si>
   <si>
-    <t>Grandal</t>
-  </si>
-  <si>
     <t>Bellinger</t>
   </si>
   <si>
-    <t>Puig</t>
-  </si>
-  <si>
-    <t>St. Louis Cardinals righties</t>
-  </si>
-  <si>
-    <t>Bader</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>Ozuna</t>
-  </si>
-  <si>
-    <t>New York Yankees hitters</t>
-  </si>
-  <si>
-    <t>Gardner</t>
-  </si>
-  <si>
-    <t>Hicks</t>
-  </si>
-  <si>
-    <t>Walker</t>
-  </si>
-  <si>
-    <t>Andujar</t>
+    <t>Pittsburgh Pirates lefties</t>
+  </si>
+  <si>
+    <t>Frazier</t>
+  </si>
+  <si>
+    <t>Polanco</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>Moran</t>
+  </si>
+  <si>
+    <t>Los Angeles Dodgers hitters</t>
+  </si>
+  <si>
+    <t>Utley</t>
+  </si>
+  <si>
+    <t>Muncy</t>
+  </si>
+  <si>
+    <t>Milwaukee Brewers righties</t>
+  </si>
+  <si>
+    <t>Cain</t>
+  </si>
+  <si>
+    <t>Braun</t>
+  </si>
+  <si>
+    <t>Santana</t>
+  </si>
+  <si>
+    <t>Perez</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,13 +502,13 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="F1" s="10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
@@ -560,7 +557,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="5">
-        <v>2400</v>
+        <v>2200</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -570,30 +567,30 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5">
-        <v>3700</v>
+        <v>4300</v>
       </c>
       <c r="H3">
-        <v>28.2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>7.6216216216216219</v>
+        <v>0.69767441860465118</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L3" s="5">
-        <v>3200</v>
+        <v>2500</v>
       </c>
       <c r="M3">
-        <v>15.2</v>
+        <v>0</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>4.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -601,40 +598,41 @@
         <v>12</v>
       </c>
       <c r="B4" s="5">
-        <v>3100</v>
+        <v>3500</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <f>6.2+18.7</f>
+        <v>24.9</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>0</v>
+        <v>7.1142857142857139</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G4" s="5">
-        <v>2800</v>
+        <v>3500</v>
       </c>
       <c r="H4">
-        <v>18.7</v>
+        <v>3</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>6.6785714285714288</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="L4" s="5">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>0</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -642,40 +640,40 @@
         <v>13</v>
       </c>
       <c r="B5" s="5">
-        <v>3400</v>
+        <v>3200</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>2.6470588235294117</v>
+        <v>3.0312499999999996</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" s="5">
-        <v>3400</v>
+        <v>3100</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>0.88235294117647067</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="L5" s="5">
-        <v>2600</v>
+        <v>3300</v>
       </c>
       <c r="M5">
-        <v>3</v>
+        <v>18.7</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>1.153846153846154</v>
+        <v>5.6666666666666661</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -683,41 +681,40 @@
         <v>14</v>
       </c>
       <c r="B6" s="5">
-        <v>2700</v>
+        <v>3100</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.967741935483871</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" s="5">
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="H6">
-        <f>18.7+6.2+6.2</f>
-        <v>31.099999999999998</v>
+        <v>3</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>11.107142857142858</v>
+        <v>0.9375</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L6" s="5">
-        <v>2700</v>
+        <v>2200</v>
       </c>
       <c r="M6">
-        <v>9.4</v>
+        <v>9.5</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>3.4814814814814818</v>
+        <v>4.3181818181818183</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -726,57 +723,53 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>11600</v>
+        <v>12000</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>9</v>
+        <v>37.599999999999994</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>0.77586206896551724</v>
+        <v>3.1333333333333329</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>12700</v>
+        <v>14100</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>6.377952755905512</v>
+        <v>0.85106382978723405</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>11500</v>
+        <v>10500</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>27.6</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>2.4000000000000004</v>
+        <v>3.5904761904761906</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="D8" s="8"/>
       <c r="I8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
@@ -909,7 +902,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3">
         <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>3.2849162011173183</v>
+        <v>2.3852459016393444</v>
       </c>
     </row>
   </sheetData>
@@ -942,19 +935,19 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Los Angeles Dodgers lefties|Pederson, Grandal, Bellinger, Puig|$11,600|9|0.78x|Failure|</v>
+        <v>|Pittsburgh Pirates lefties|Frazier, Polanco, Bell, Moran|$12,000|37.6|3.13x||</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|St. Louis Cardinals righties|Pham, Bader, Martinez, Ozuna|$12,700|81|6.38x|Success|</v>
+        <v>|Milwaukee Brewers righties|Cain, Braun, Santana, Perez|$14,100|12|0.85x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|New York Yankees hitters|Gardner, Hicks, Walker, Andujar|$11,500|27.6|2.4x|Failure|</v>
+        <v>|Los Angeles Dodgers hitters|Utley, Pederson, Bellinger, Muncy|$10,500|37.7|3.59x||</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adjusted weights for recent player performance
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Player</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
   <si>
     <t>Failure</t>
@@ -480,7 +483,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,19 +499,19 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="F1" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
@@ -554,7 +557,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5">
         <v>2200</v>
@@ -567,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5">
         <v>4300</v>
@@ -580,7 +583,7 @@
         <v>0.69767441860465118</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L3" s="5">
         <v>2500</v>
@@ -595,7 +598,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5">
         <v>3500</v>
@@ -609,7 +612,7 @@
         <v>7.1142857142857139</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5">
         <v>3500</v>
@@ -622,7 +625,7 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="K4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L4" s="5">
         <v>2500</v>
@@ -637,20 +640,20 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5">
         <v>3200</v>
       </c>
       <c r="C5">
-        <v>9.6999999999999993</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>3.0312499999999996</v>
+        <v>5.9062499999999991</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="5">
         <v>3100</v>
@@ -663,7 +666,7 @@
         <v>0.967741935483871</v>
       </c>
       <c r="K5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L5" s="5">
         <v>3300</v>
@@ -678,7 +681,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5">
         <v>3100</v>
@@ -691,7 +694,7 @@
         <v>0.967741935483871</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5">
         <v>3200</v>
@@ -704,17 +707,17 @@
         <v>0.9375</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6" s="5">
         <v>2200</v>
       </c>
       <c r="M6">
-        <v>9.5</v>
+        <v>12.5</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>4.3181818181818183</v>
+        <v>5.6818181818181817</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -727,11 +730,11 @@
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>37.599999999999994</v>
+        <v>46.8</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>3.1333333333333329</v>
+        <v>3.9</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -757,19 +760,23 @@
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>37.700000000000003</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>3.5904761904761906</v>
+        <v>3.8761904761904766</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="I8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
@@ -902,7 +909,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3">
         <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>2.3852459016393444</v>
+        <v>2.7185792349726778</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +942,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Pittsburgh Pirates lefties|Frazier, Polanco, Bell, Moran|$12,000|37.6|3.13x||</v>
+        <v>|Pittsburgh Pirates lefties|Frazier, Polanco, Bell, Moran|$12,000|46.8|3.9x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -947,7 +954,7 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Los Angeles Dodgers hitters|Utley, Pederson, Bellinger, Muncy|$10,500|37.7|3.59x||</v>
+        <v>|Los Angeles Dodgers hitters|Utley, Pederson, Bellinger, Muncy|$10,500|40.7|3.88x|Success|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Choose separate stacks for FD vs DK
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Player</t>
   </si>
@@ -48,55 +48,70 @@
     <t>???</t>
   </si>
   <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Los Angeles Dodgers hitters</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Pittsburgh Pirates lefties</t>
+  </si>
+  <si>
+    <t>Frazier</t>
+  </si>
+  <si>
+    <t>Polanco</t>
+  </si>
+  <si>
+    <t>Dickerson</t>
+  </si>
+  <si>
+    <t>Moran</t>
+  </si>
+  <si>
+    <t>Kansas City Royals righties</t>
+  </si>
+  <si>
+    <t>Merrifield</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>Escobar</t>
+  </si>
+  <si>
+    <t>Almonte</t>
+  </si>
+  <si>
+    <t>Detroit Tigers hitters</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Kozma</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Goodrum</t>
+  </si>
+  <si>
+    <t>Hernandez (INJ)</t>
+  </si>
+  <si>
+    <t>Barnes (INJ)</t>
+  </si>
+  <si>
     <t>Success</t>
-  </si>
-  <si>
-    <t>Failure</t>
-  </si>
-  <si>
-    <t>Pederson</t>
-  </si>
-  <si>
-    <t>Bellinger</t>
-  </si>
-  <si>
-    <t>Pittsburgh Pirates lefties</t>
-  </si>
-  <si>
-    <t>Frazier</t>
-  </si>
-  <si>
-    <t>Polanco</t>
-  </si>
-  <si>
-    <t>Bell</t>
-  </si>
-  <si>
-    <t>Moran</t>
-  </si>
-  <si>
-    <t>Los Angeles Dodgers hitters</t>
-  </si>
-  <si>
-    <t>Utley</t>
-  </si>
-  <si>
-    <t>Muncy</t>
-  </si>
-  <si>
-    <t>Milwaukee Brewers righties</t>
-  </si>
-  <si>
-    <t>Cain</t>
-  </si>
-  <si>
-    <t>Braun</t>
-  </si>
-  <si>
-    <t>Santana</t>
-  </si>
-  <si>
-    <t>Perez</t>
   </si>
 </sst>
 </file>
@@ -483,12 +498,12 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -499,13 +514,13 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="F1" s="10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -557,167 +572,166 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5">
-        <v>2200</v>
+        <v>3600</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G3" s="5">
-        <v>4300</v>
+        <v>2100</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>24.9</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>0.69767441860465118</v>
+        <v>11.857142857142856</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
       </c>
       <c r="L3" s="5">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>0</v>
+        <v>4.7142857142857144</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5">
-        <v>3500</v>
+        <v>2400</v>
       </c>
       <c r="C4">
-        <f>6.2+18.7</f>
-        <v>24.9</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>7.1142857142857139</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5">
         <v>3500</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>21.9</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>0.8571428571428571</v>
+        <v>6.2571428571428571</v>
       </c>
       <c r="K4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="L4" s="5">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="M4">
-        <v>9.5</v>
+        <v>0</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>3.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
-        <v>3200</v>
+        <v>3000</v>
       </c>
       <c r="C5">
-        <v>18.899999999999999</v>
+        <v>3</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>5.9062499999999991</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5">
-        <v>3100</v>
+        <v>3900</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>0.967741935483871</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="L5" s="5">
-        <v>3300</v>
+        <v>2100</v>
       </c>
       <c r="M5">
-        <v>18.7</v>
+        <v>6</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>5.6666666666666661</v>
+        <v>2.8571428571428572</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5">
-        <v>3100</v>
+        <v>2200</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>0.967741935483871</v>
+        <v>1.3636363636363638</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G6" s="5">
-        <v>3200</v>
+        <v>2800</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>15.5</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>5.5357142857142856</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5">
-        <v>2200</v>
+        <v>2100</v>
       </c>
       <c r="M6">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>5.6818181818181817</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -726,45 +740,45 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>12000</v>
+        <v>11200</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>46.8</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>3.9</v>
+        <v>1.0714285714285714</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>14100</v>
+        <v>12300</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>12</v>
+        <v>65.3</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>0.85106382978723405</v>
+        <v>5.308943089430894</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>10500</v>
+        <v>11200</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>40.700000000000003</v>
+        <v>22.5</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>3.8761904761904766</v>
+        <v>2.0089285714285712</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -772,14 +786,16 @@
         <v>7</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="N8" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -815,10 +831,18 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="D11" s="7" t="e">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C11">
+        <v>31.4</v>
+      </c>
+      <c r="D11" s="7">
         <f>(C11 / B11) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>12.56</v>
       </c>
       <c r="G11" s="5"/>
       <c r="I11" s="7" t="e">
@@ -827,10 +851,18 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="D12" s="7" t="e">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2600</v>
+      </c>
+      <c r="C12">
+        <v>12.7</v>
+      </c>
+      <c r="D12" s="7">
         <f t="shared" ref="D12:D13" si="3">(C12 / B12) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>4.8846153846153841</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="7" t="e">
@@ -839,10 +871,18 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="D13" s="7" t="e">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2400</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.25</v>
       </c>
       <c r="G13" s="5"/>
       <c r="I13" s="7" t="e">
@@ -851,10 +891,18 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="D14" s="7" t="e">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C14">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D14" s="7">
         <f>(C14 / B14) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>3.6799999999999997</v>
       </c>
       <c r="G14" s="5"/>
       <c r="I14" s="7" t="e">
@@ -868,15 +916,15 @@
       </c>
       <c r="B15" s="6">
         <f>SUM(B11:B14)</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="C15" s="1">
         <f>SUM(C11:C14)</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="3" t="e">
+        <v>56.3</v>
+      </c>
+      <c r="D15" s="3">
         <f>(C15 / B15) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>5.63</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>4</v>
@@ -896,7 +944,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16" s="8" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>6</v>
@@ -909,7 +957,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3">
         <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>2.7185792349726778</v>
+        <v>3.4921700223713645</v>
       </c>
     </row>
   </sheetData>
@@ -942,25 +990,25 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Pittsburgh Pirates lefties|Frazier, Polanco, Bell, Moran|$12,000|46.8|3.9x|Success|</v>
+        <v>|Los Angeles Dodgers hitters|Taylor, Hernandez (INJ), Turner, Barnes (INJ)|$11,200|12|1.07x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Milwaukee Brewers righties|Cain, Braun, Santana, Perez|$14,100|12|0.85x|Failure|</v>
+        <v>|Pittsburgh Pirates lefties|Frazier, Polanco, Dickerson, Moran|$12,300|65.3|5.31x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Los Angeles Dodgers hitters|Utley, Pederson, Bellinger, Muncy|$10,500|40.7|3.88x|Success|</v>
+        <v>|Kansas City Royals righties|Merrifield, Perez, Escobar, Almonte|$11,200|22.5|2.01x|Failure|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="e">
+      <c r="A4" t="str">
         <f>CONCATENATE("|",Sheet1!A9,"|",Sheet1!A11,", ",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,"|",TEXT(Sheet1!B15,"$#,##0"),"|",Sheet1!C15,"|",CONCATENATE(ROUND(Sheet1!D15,2),"x"),"|",Sheet1!D16,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Detroit Tigers hitters|Jones, Kozma, Martinez, Goodrum|$10,000|56.3|5.63x|Success|</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added "Suspended" game status
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
   <si>
     <t>Player</t>
   </si>
@@ -40,78 +40,6 @@
   </si>
   <si>
     <t>Total:</t>
-  </si>
-  <si>
-    <t>Overall value:</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Failure</t>
-  </si>
-  <si>
-    <t>Los Angeles Dodgers hitters</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Turner</t>
-  </si>
-  <si>
-    <t>Pittsburgh Pirates lefties</t>
-  </si>
-  <si>
-    <t>Frazier</t>
-  </si>
-  <si>
-    <t>Polanco</t>
-  </si>
-  <si>
-    <t>Dickerson</t>
-  </si>
-  <si>
-    <t>Moran</t>
-  </si>
-  <si>
-    <t>Kansas City Royals righties</t>
-  </si>
-  <si>
-    <t>Merrifield</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>Escobar</t>
-  </si>
-  <si>
-    <t>Almonte</t>
-  </si>
-  <si>
-    <t>Detroit Tigers hitters</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Kozma</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>Goodrum</t>
-  </si>
-  <si>
-    <t>Hernandez (INJ)</t>
-  </si>
-  <si>
-    <t>Barnes (INJ)</t>
-  </si>
-  <si>
-    <t>Success</t>
   </si>
 </sst>
 </file>
@@ -203,10 +131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -495,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,24 +441,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="F1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="K1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -571,167 +493,71 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5">
-        <v>3600</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="B3" s="5"/>
+      <c r="D3" s="7" t="e">
         <f>(C3 / B3) * 1000</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5">
-        <v>2100</v>
-      </c>
-      <c r="H3">
-        <v>24.9</v>
-      </c>
-      <c r="I3" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="I3" s="7" t="e">
         <f>(H3 / G3) * 1000</f>
-        <v>11.857142857142856</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="5">
-        <v>3500</v>
-      </c>
-      <c r="M3">
-        <v>16.5</v>
-      </c>
-      <c r="N3" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="N3" s="7" t="e">
         <f>(M3 / L3) * 1000</f>
-        <v>4.7142857142857144</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2400</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="B4" s="5"/>
+      <c r="D4" s="7" t="e">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5">
-        <v>3500</v>
-      </c>
-      <c r="H4">
-        <v>21.9</v>
-      </c>
-      <c r="I4" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="I4" s="7" t="e">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>6.2571428571428571</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="5">
-        <v>3500</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="N4" s="7" t="e">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3000</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="B5" s="5"/>
+      <c r="D5" s="7" t="e">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3900</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="I5" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>0.76923076923076927</v>
-      </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="5">
-        <v>2100</v>
-      </c>
-      <c r="M5">
-        <v>6</v>
-      </c>
-      <c r="N5" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="N5" s="7" t="e">
         <f t="shared" si="2"/>
-        <v>2.8571428571428572</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2200</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="5"/>
+      <c r="D6" s="7" t="e">
         <f t="shared" si="0"/>
-        <v>1.3636363636363638</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2800</v>
-      </c>
-      <c r="H6">
-        <v>15.5</v>
-      </c>
-      <c r="I6" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="I6" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>5.5357142857142856</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="5">
-        <v>2100</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="N6" s="7" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -740,234 +566,237 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>11200</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>12</v>
-      </c>
-      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>1.0714285714285714</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>12300</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>65.3</v>
-      </c>
-      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="e">
         <f t="shared" si="1"/>
-        <v>5.308943089430894</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>11200</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>22.5</v>
-      </c>
-      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3" t="e">
         <f t="shared" si="2"/>
-        <v>2.0089285714285712</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="D8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
       <c r="I9" s="10"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5">
-        <v>2500</v>
-      </c>
-      <c r="C11">
-        <v>31.4</v>
-      </c>
-      <c r="D11" s="7">
-        <f>(C11 / B11) * 1000</f>
-        <v>12.56</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="I11" s="7" t="e">
-        <f>(H11 / G11) * 1000</f>
-        <v>#DIV/0!</v>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="5">
-        <v>2600</v>
-      </c>
-      <c r="C12">
-        <v>12.7</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" ref="D12:D13" si="3">(C12 / B12) * 1000</f>
-        <v>4.8846153846153841</v>
+      <c r="B12" s="5"/>
+      <c r="D12" s="7" t="e">
+        <f>(C12 / B12) * 1000</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="7" t="e">
-        <f t="shared" ref="I12:I13" si="4">(H12 / G12) * 1000</f>
+        <f>(H12 / G12) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="N12" s="7" t="e">
+        <f>(M12 / L12) * 1000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2400</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="3"/>
-        <v>1.25</v>
+      <c r="B13" s="5"/>
+      <c r="D13" s="7" t="e">
+        <f t="shared" ref="D13:D14" si="3">(C13 / B13) * 1000</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="G13" s="5"/>
       <c r="I13" s="7" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I13:I14" si="4">(H13 / G13) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="N13" s="7" t="e">
+        <f t="shared" ref="N13:N14" si="5">(M13 / L13) * 1000</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2500</v>
-      </c>
-      <c r="C14">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D14" s="7">
-        <f>(C14 / B14) * 1000</f>
-        <v>3.6799999999999997</v>
+      <c r="B14" s="5"/>
+      <c r="D14" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="G14" s="5"/>
       <c r="I14" s="7" t="e">
-        <f>(H14 / G14) * 1000</f>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="N14" s="7" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="5"/>
+      <c r="D15" s="7" t="e">
+        <f>(C15 / B15) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="I15" s="7" t="e">
+        <f>(H15 / G15) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="N15" s="7" t="e">
+        <f>(M15 / L15) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="6">
-        <f>SUM(B11:B14)</f>
-        <v>10000</v>
-      </c>
-      <c r="C15" s="1">
-        <f>SUM(C11:C14)</f>
-        <v>56.3</v>
-      </c>
-      <c r="D15" s="3">
-        <f>(C15 / B15) * 1000</f>
-        <v>5.63</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="B16" s="6">
+        <f>SUM(B12:B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUM(C12:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="e">
+        <f>(C16 / B16) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="6">
-        <f>SUM(G11:G14)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <f>SUM(H11:H14)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="3" t="e">
-        <f>(H15 / G15) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="3">
-        <f>(SUM(C7,H7,M7, C15,H15) / SUM(B7,G7,L7,B15,G15)) * 1000</f>
-        <v>3.4921700223713645</v>
-      </c>
+      <c r="G16" s="6">
+        <f>SUM(G12:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SUM(H12:H15)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="e">
+        <f>(H16 / G16) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="6">
+        <f>SUM(L12:L15)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f>SUM(M12:M15)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3" t="e">
+        <f>(M16 / L16) * 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -976,10 +805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,32 +817,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
+      <c r="A1" t="e">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Los Angeles Dodgers hitters|Taylor, Hernandez (INJ), Turner, Barnes (INJ)|$11,200|12|1.07x|Failure|</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+      <c r="A2" t="e">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Pittsburgh Pirates lefties|Frazier, Polanco, Dickerson, Moran|$12,300|65.3|5.31x|Success|</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+      <c r="A3" t="e">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Kansas City Royals righties|Merrifield, Perez, Escobar, Almonte|$11,200|22.5|2.01x|Failure|</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>CONCATENATE("|",Sheet1!A9,"|",Sheet1!A11,", ",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,"|",TEXT(Sheet1!B15,"$#,##0"),"|",Sheet1!C15,"|",CONCATENATE(ROUND(Sheet1!D15,2),"x"),"|",Sheet1!D16,"|")</f>
-        <v>|Detroit Tigers hitters|Jones, Kozma, Martinez, Goodrum|$10,000|56.3|5.63x|Success|</v>
+      <c r="A4" t="e">
+        <f>CONCATENATE("|",Sheet1!A10,"|",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,", ",Sheet1!A15,"|",TEXT(Sheet1!B16,"$#,##0"),"|",Sheet1!C16,"|",CONCATENATE(ROUND(Sheet1!D16,2),"x"),"|",Sheet1!D17,"|")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="e">
-        <f>CONCATENATE("|",Sheet1!F9,"|",Sheet1!F11,", ",Sheet1!F12,", ",Sheet1!F13,", ",Sheet1!F14,"|",TEXT(Sheet1!G15,"$#,##0"),"|",Sheet1!H15,"|",CONCATENATE(ROUND(Sheet1!I15,2),"x"),"|",Sheet1!I16,"|")</f>
+        <f>CONCATENATE("|",Sheet1!F10,"|",Sheet1!F12,", ",Sheet1!F13,", ",Sheet1!F14,", ",Sheet1!F15,"|",TEXT(Sheet1!G16,"$#,##0"),"|",Sheet1!H16,"|",CONCATENATE(ROUND(Sheet1!I16,2),"x"),"|",Sheet1!I17,"|")</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="e">
+        <f>CONCATENATE("|",Sheet1!K10,"|",Sheet1!K12,", ",Sheet1!K13,", ",Sheet1!K14,", ",Sheet1!K15,"|",TEXT(Sheet1!L16,"$#,##0"),"|",Sheet1!M16,"|",CONCATENATE(ROUND(Sheet1!N16,2),"x"),"|",Sheet1!N17,"|")</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Choose stacks by proj FPTS + value (instead of just value);  Load games & players from start of 2017
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>Player</t>
   </si>
@@ -40,6 +40,72 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>Toronto Blue Jays hitters (FD)</t>
+  </si>
+  <si>
+    <t>Chicago White Sox hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Detroit Tigers righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Colorado Rockies lefties (FD)</t>
+  </si>
+  <si>
+    <t>Granderson</t>
+  </si>
+  <si>
+    <t>Smoak</t>
+  </si>
+  <si>
+    <t>Pillar</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Moncada</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Delmonico</t>
+  </si>
+  <si>
+    <t>Castillo</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Kozma</t>
+  </si>
+  <si>
+    <t>Castellanos</t>
+  </si>
+  <si>
+    <t>Mahtook</t>
+  </si>
+  <si>
+    <t>Blackmon</t>
+  </si>
+  <si>
+    <t>Parra</t>
+  </si>
+  <si>
+    <t>Wolters</t>
   </si>
 </sst>
 </file>
@@ -426,7 +492,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,15 +507,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -493,71 +565,167 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="D3" s="7" t="e">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C3">
+        <v>15.7</v>
+      </c>
+      <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="7" t="e">
+        <v>6.28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3600</v>
+      </c>
+      <c r="H3">
+        <v>15.2</v>
+      </c>
+      <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="N3" s="7" t="e">
+        <v>4.2222222222222214</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2700</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="D4" s="7" t="e">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3400</v>
+      </c>
+      <c r="C4">
+        <v>15.7</v>
+      </c>
+      <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="I4" s="7" t="e">
+        <v>4.617647058823529</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2800</v>
+      </c>
+      <c r="H4">
+        <v>3.2</v>
+      </c>
+      <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="N4" s="7" t="e">
+        <v>1.142857142857143</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="5">
+        <v>2800</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="D5" s="7" t="e">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2900</v>
+      </c>
+      <c r="C5">
+        <v>15.7</v>
+      </c>
+      <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="I5" s="7" t="e">
+        <v>5.4137931034482749</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2500</v>
+      </c>
+      <c r="H5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="N5" s="7" t="e">
+        <v>3.88</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3600</v>
+      </c>
+      <c r="M5">
+        <v>9</v>
+      </c>
+      <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="D6" s="7" t="e">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="I6" s="7" t="e">
+        <v>3.6799999999999997</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2300</v>
+      </c>
+      <c r="H6">
+        <v>10.5</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="N6" s="7" t="e">
+        <v>4.5652173913043486</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="5">
+        <v>2200</v>
+      </c>
+      <c r="M6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>4.1818181818181817</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -566,51 +734,57 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>0</v>
+        <v>11300</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="e">
+        <v>56.3</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>4.9823008849557517</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>0</v>
+        <v>11200</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="e">
+        <v>38.599999999999994</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>3.4464285714285707</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>0</v>
+        <v>11300</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="3" t="e">
+        <v>18.2</v>
+      </c>
+      <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.6106194690265487</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="10"/>
@@ -618,7 +792,9 @@
       <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -670,10 +846,18 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="D12" s="7" t="e">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5">
+        <v>4300</v>
+      </c>
+      <c r="C12">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D12" s="7">
         <f>(C12 / B12) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>2.13953488372093</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="7" t="e">
@@ -687,10 +871,18 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="D13" s="7" t="e">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2600</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7">
         <f t="shared" ref="D13:D14" si="3">(C13 / B13) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>2.3076923076923079</v>
       </c>
       <c r="G13" s="5"/>
       <c r="I13" s="7" t="e">
@@ -704,10 +896,18 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="D14" s="7" t="e">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2700</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>4.8148148148148149</v>
       </c>
       <c r="G14" s="5"/>
       <c r="I14" s="7" t="e">
@@ -721,10 +921,18 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="D15" s="7" t="e">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2000</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
         <f>(C15 / B15) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5"/>
       <c r="I15" s="7" t="e">
@@ -743,15 +951,15 @@
       </c>
       <c r="B16" s="6">
         <f>SUM(B12:B15)</f>
-        <v>0</v>
+        <v>11600</v>
       </c>
       <c r="C16" s="1">
         <f>SUM(C12:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="e">
+        <v>28.2</v>
+      </c>
+      <c r="D16" s="3">
         <f>(C16 / B16) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>2.4310344827586206</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>4</v>
@@ -785,7 +993,9 @@
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="N17" s="8"/>
     </row>
@@ -817,27 +1027,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="e">
+      <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Toronto Blue Jays hitters (FD)|Granderson, Smoak, Pillar, Martin|$11,300|56.3|4.98x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
+      <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Chicago White Sox hitters (FD, DK)|Moncada, Sanchez, Delmonico, Castillo|$11,200|38.6|3.45x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="e">
+      <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Detroit Tigers righties (FD, DK)|Jones, Kozma, Castellanos, Mahtook|$11,300|18.2|1.61x|Failure|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="e">
+      <c r="A4" t="str">
         <f>CONCATENATE("|",Sheet1!A10,"|",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,", ",Sheet1!A15,"|",TEXT(Sheet1!B16,"$#,##0"),"|",Sheet1!C16,"|",CONCATENATE(ROUND(Sheet1!D16,2),"x"),"|",Sheet1!D17,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Colorado Rockies lefties (FD)|Blackmon, Parra, Gonzalez, Wolters|$11,600|28.2|2.43x|Failure|</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Draftbook enhancement to not show FPTS/PA stats for pitchers not playing on a given DFS site
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Player</t>
   </si>
@@ -48,64 +48,61 @@
     <t>Success</t>
   </si>
   <si>
+    <t>Palka</t>
+  </si>
+  <si>
+    <t>DeShields</t>
+  </si>
+  <si>
+    <t>Kiner-Falefa</t>
+  </si>
+  <si>
+    <t>Choo</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>Blackmon</t>
+  </si>
+  <si>
+    <t>Dahl</t>
+  </si>
+  <si>
+    <t>Milwaukee Brewers lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Yelich</t>
+  </si>
+  <si>
+    <t>Shaw</t>
+  </si>
+  <si>
+    <t>Villar</t>
+  </si>
+  <si>
+    <t>Texas Rangers hitters (DK)</t>
+  </si>
+  <si>
+    <t>Gallo</t>
+  </si>
+  <si>
+    <t>Colorado Rockies lefties (DK)</t>
+  </si>
+  <si>
     <t>Gonzalez</t>
   </si>
   <si>
-    <t>Toronto Blue Jays hitters (FD)</t>
-  </si>
-  <si>
     <t>Chicago White Sox hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Detroit Tigers righties (FD, DK)</t>
-  </si>
-  <si>
-    <t>Colorado Rockies lefties (FD)</t>
-  </si>
-  <si>
-    <t>Granderson</t>
-  </si>
-  <si>
-    <t>Smoak</t>
-  </si>
-  <si>
-    <t>Pillar</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>Moncada</t>
-  </si>
-  <si>
-    <t>Sanchez</t>
-  </si>
-  <si>
-    <t>Delmonico</t>
-  </si>
-  <si>
-    <t>Castillo</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Kozma</t>
-  </si>
-  <si>
-    <t>Castellanos</t>
-  </si>
-  <si>
-    <t>Mahtook</t>
-  </si>
-  <si>
-    <t>Blackmon</t>
-  </si>
-  <si>
-    <t>Parra</t>
-  </si>
-  <si>
-    <t>Wolters</t>
+    <t>Abreu</t>
+  </si>
+  <si>
+    <t>Rondon</t>
   </si>
 </sst>
 </file>
@@ -197,10 +194,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,24 +504,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="A1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="K1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -566,166 +563,150 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" s="5">
-        <v>2500</v>
+        <v>3300</v>
       </c>
       <c r="C3">
-        <v>15.7</v>
+        <v>15.4</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>6.28</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5">
-        <v>3600</v>
+        <v>5600</v>
       </c>
       <c r="H3">
-        <v>15.2</v>
+        <v>10</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>4.2222222222222214</v>
+        <v>1.7857142857142856</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L3" s="5">
-        <v>2700</v>
+        <v>3300</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>0</v>
+        <v>3.0303030303030303</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B4" s="5">
-        <v>3400</v>
+        <v>3700</v>
       </c>
       <c r="C4">
-        <v>15.7</v>
+        <v>12.7</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>4.617647058823529</v>
+        <v>3.4324324324324325</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" s="5">
-        <v>2800</v>
+        <v>4000</v>
       </c>
       <c r="H4">
-        <v>3.2</v>
+        <v>14</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>1.142857142857143</v>
+        <v>3.5</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="L4" s="5">
-        <v>2800</v>
+        <v>4100</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>0</v>
+        <v>1.7073170731707317</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5">
-        <v>2900</v>
+        <v>2400</v>
       </c>
       <c r="C5">
-        <v>15.7</v>
+        <v>9.5</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>5.4137931034482749</v>
+        <v>3.9583333333333335</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" s="5">
-        <v>2500</v>
+        <v>3600</v>
       </c>
       <c r="H5">
-        <v>9.6999999999999993</v>
+        <v>27</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>3.88</v>
+        <v>7.5</v>
       </c>
       <c r="K5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="L5" s="5">
-        <v>3600</v>
+        <v>3500</v>
       </c>
       <c r="M5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2500</v>
-      </c>
-      <c r="C6">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="5"/>
+      <c r="D6" s="7" t="e">
         <f t="shared" si="0"/>
-        <v>3.6799999999999997</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2300</v>
-      </c>
-      <c r="H6">
-        <v>10.5</v>
-      </c>
-      <c r="I6" s="7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="I6" s="7" t="e">
         <f t="shared" si="1"/>
-        <v>4.5652173913043486</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5">
-        <v>2200</v>
+        <v>3800</v>
       </c>
       <c r="M6">
-        <v>9.1999999999999993</v>
+        <v>14</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>4.1818181818181817</v>
+        <v>3.6842105263157894</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -734,45 +715,45 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>11300</v>
+        <v>9400</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>56.3</v>
+        <v>37.6</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>4.9823008849557517</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>11200</v>
+        <v>13200</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>38.599999999999994</v>
+        <v>51</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>3.4464285714285707</v>
+        <v>3.8636363636363638</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>11300</v>
+        <v>14700</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>18.2</v>
+        <v>34</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>1.6106194690265487</v>
+        <v>2.3129251700680271</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -780,32 +761,32 @@
         <v>6</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
+      <c r="A10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -847,17 +828,17 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>4300</v>
+        <v>3000</v>
       </c>
       <c r="C12">
-        <v>9.1999999999999993</v>
+        <v>6.2</v>
       </c>
       <c r="D12" s="7">
         <f>(C12 / B12) * 1000</f>
-        <v>2.13953488372093</v>
+        <v>2.0666666666666669</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="7" t="e">
@@ -872,17 +853,17 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5">
-        <v>2600</v>
+        <v>3800</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" ref="D13:D14" si="3">(C13 / B13) * 1000</f>
-        <v>2.3076923076923079</v>
+        <v>0</v>
       </c>
       <c r="G13" s="5"/>
       <c r="I13" s="7" t="e">
@@ -897,17 +878,17 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5">
-        <v>2700</v>
+        <v>2900</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>18.7</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" si="3"/>
-        <v>4.8148148148148149</v>
+        <v>6.4482758620689653</v>
       </c>
       <c r="G14" s="5"/>
       <c r="I14" s="7" t="e">
@@ -922,17 +903,17 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B15" s="5">
-        <v>2000</v>
+        <v>2900</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D15" s="7">
         <f>(C15 / B15) * 1000</f>
-        <v>0</v>
+        <v>4.1379310344827589</v>
       </c>
       <c r="G15" s="5"/>
       <c r="I15" s="7" t="e">
@@ -951,27 +932,19 @@
       </c>
       <c r="B16" s="6">
         <f>SUM(B12:B15)</f>
-        <v>11600</v>
+        <v>12600</v>
       </c>
       <c r="C16" s="1">
         <f>SUM(C12:C15)</f>
-        <v>28.2</v>
+        <v>36.9</v>
       </c>
       <c r="D16" s="3">
         <f>(C16 / B16) * 1000</f>
-        <v>2.4310344827586206</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="6">
-        <f>SUM(G12:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <f>SUM(H12:H15)</f>
-        <v>0</v>
-      </c>
+        <v>2.9285714285714284</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="3" t="e">
         <f>(H16 / G16) * 1000</f>
         <v>#DIV/0!</v>
@@ -998,6 +971,11 @@
       </c>
       <c r="I17" s="8"/>
       <c r="N17" s="8"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1018,7 +996,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,25 +1007,25 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Toronto Blue Jays hitters (FD)|Granderson, Smoak, Pillar, Martin|$11,300|56.3|4.98x|Success|</v>
+        <v>|Milwaukee Brewers lefties (FD, DK)|Yelich, Shaw, Villar, |$9,400|37.6|4x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Chicago White Sox hitters (FD, DK)|Moncada, Sanchez, Delmonico, Castillo|$11,200|38.6|3.45x|Failure|</v>
+        <v>|Colorado Rockies lefties (DK)|Blackmon, Dahl, Gonzalez, |$13,200|51|3.86x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Detroit Tigers righties (FD, DK)|Jones, Kozma, Castellanos, Mahtook|$11,300|18.2|1.61x|Failure|</v>
+        <v>|Texas Rangers hitters (DK)|DeShields, Choo, Kiner-Falefa, Gallo|$14,700|34|2.31x|Success|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE("|",Sheet1!A10,"|",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,", ",Sheet1!A15,"|",TEXT(Sheet1!B16,"$#,##0"),"|",Sheet1!C16,"|",CONCATENATE(ROUND(Sheet1!D16,2),"x"),"|",Sheet1!D17,"|")</f>
-        <v>|Colorado Rockies lefties (FD)|Blackmon, Parra, Gonzalez, Wolters|$11,600|28.2|2.43x|Failure|</v>
+        <v>|Chicago White Sox hitters (FD, DK)|Anderson, Abreu, Rondon, Palka|$12,600|36.9|2.93x|Failure|</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Error handling fix to handle pitchers who also start as hitters (e.g. Ohtani)
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Player</t>
   </si>
@@ -45,64 +45,52 @@
     <t>Failure</t>
   </si>
   <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Palka</t>
-  </si>
-  <si>
-    <t>DeShields</t>
-  </si>
-  <si>
-    <t>Kiner-Falefa</t>
-  </si>
-  <si>
-    <t>Choo</t>
-  </si>
-  <si>
-    <t>Anderson</t>
-  </si>
-  <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t>Blackmon</t>
-  </si>
-  <si>
-    <t>Dahl</t>
-  </si>
-  <si>
-    <t>Milwaukee Brewers lefties (FD, DK)</t>
-  </si>
-  <si>
-    <t>Yelich</t>
-  </si>
-  <si>
-    <t>Shaw</t>
-  </si>
-  <si>
-    <t>Villar</t>
-  </si>
-  <si>
-    <t>Texas Rangers hitters (DK)</t>
-  </si>
-  <si>
-    <t>Gallo</t>
-  </si>
-  <si>
-    <t>Colorado Rockies lefties (DK)</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
-    <t>Chicago White Sox hitters (FD, DK)</t>
-  </si>
-  <si>
-    <t>Abreu</t>
-  </si>
-  <si>
-    <t>Rondon</t>
+    <t>Colorado Rockies righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Desmond</t>
+  </si>
+  <si>
+    <t>Arenado</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Cuevas</t>
+  </si>
+  <si>
+    <t>Seattle Mariners hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Atlanta Braves hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Segura</t>
+  </si>
+  <si>
+    <t>Heredia</t>
+  </si>
+  <si>
+    <t>Haniger</t>
+  </si>
+  <si>
+    <t>Healy</t>
+  </si>
+  <si>
+    <t>Inciarte</t>
+  </si>
+  <si>
+    <t>Freeman</t>
+  </si>
+  <si>
+    <t>Markakis</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
   </si>
 </sst>
 </file>
@@ -489,7 +477,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,19 +493,19 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="F1" s="10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
@@ -563,150 +551,166 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5">
         <v>3300</v>
       </c>
       <c r="C3">
-        <v>15.4</v>
+        <v>15.7</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>4.666666666666667</v>
+        <v>4.7575757575757569</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G3" s="5">
-        <v>5600</v>
+        <v>2800</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>1.7857142857142856</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="L3" s="5">
-        <v>3300</v>
+        <v>3000</v>
       </c>
       <c r="M3">
-        <v>10</v>
+        <v>6.2</v>
       </c>
       <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>3.0303030303030303</v>
+        <v>2.0666666666666669</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5">
-        <v>3700</v>
+        <v>2200</v>
       </c>
       <c r="C4">
-        <v>12.7</v>
+        <v>0</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:D7" si="0">(C4 / B4) * 1000</f>
-        <v>3.4324324324324325</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G4" s="5">
-        <v>4000</v>
+        <v>4300</v>
       </c>
       <c r="H4">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>3.5</v>
+        <v>1.3953488372093024</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" s="5">
-        <v>4100</v>
+        <v>5400</v>
       </c>
       <c r="M4">
-        <v>7</v>
+        <v>28.7</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>1.7073170731707317</v>
+        <v>5.3148148148148149</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5">
-        <v>2400</v>
+        <v>3500</v>
       </c>
       <c r="C5">
         <v>9.5</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>3.9583333333333335</v>
+        <v>2.7142857142857144</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5">
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="H5">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L5" s="5">
-        <v>3500</v>
+        <v>4400</v>
       </c>
       <c r="M5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="2"/>
-        <v>0.8571428571428571</v>
+        <v>1.3636363636363638</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="D6" s="7" t="e">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2800</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="I6" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2500</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="L6" s="5">
-        <v>3800</v>
+        <v>3700</v>
       </c>
       <c r="M6">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="2"/>
-        <v>3.6842105263157894</v>
+        <v>1.6216216216216215</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -715,56 +719,56 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>9400</v>
+        <v>11800</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>37.6</v>
+        <v>25.2</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2.1355932203389831</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>13200</v>
+        <v>13000</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>3.8636363636363638</v>
+        <v>0.46153846153846151</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>14700</v>
+        <v>16500</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>34</v>
+        <v>46.9</v>
       </c>
       <c r="N7" s="3">
         <f t="shared" si="2"/>
-        <v>2.3129251700680271</v>
+        <v>2.8424242424242423</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -773,9 +777,7 @@
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -827,18 +829,10 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5">
-        <v>3000</v>
-      </c>
-      <c r="C12">
-        <v>6.2</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="B12" s="5"/>
+      <c r="D12" s="7" t="e">
         <f>(C12 / B12) * 1000</f>
-        <v>2.0666666666666669</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="7" t="e">
@@ -852,18 +846,10 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5">
-        <v>3800</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="B13" s="5"/>
+      <c r="D13" s="7" t="e">
         <f t="shared" ref="D13:D14" si="3">(C13 / B13) * 1000</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G13" s="5"/>
       <c r="I13" s="7" t="e">
@@ -877,18 +863,10 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2900</v>
-      </c>
-      <c r="C14">
-        <v>18.7</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="B14" s="5"/>
+      <c r="D14" s="7" t="e">
         <f t="shared" si="3"/>
-        <v>6.4482758620689653</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G14" s="5"/>
       <c r="I14" s="7" t="e">
@@ -902,18 +880,10 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2900</v>
-      </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="B15" s="5"/>
+      <c r="D15" s="7" t="e">
         <f>(C15 / B15) * 1000</f>
-        <v>4.1379310344827589</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G15" s="5"/>
       <c r="I15" s="7" t="e">
@@ -932,19 +902,27 @@
       </c>
       <c r="B16" s="6">
         <f>SUM(B12:B15)</f>
-        <v>12600</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <f>SUM(C12:C15)</f>
-        <v>36.9</v>
-      </c>
-      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="e">
         <f>(C16 / B16) * 1000</f>
-        <v>2.9285714285714284</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="6">
+        <f>SUM(G12:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SUM(H12:H15)</f>
+        <v>0</v>
+      </c>
       <c r="I16" s="3" t="e">
         <f>(H16 / G16) * 1000</f>
         <v>#DIV/0!</v>
@@ -966,15 +944,13 @@
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="D17" s="8"/>
       <c r="I17" s="8"/>
       <c r="N17" s="8"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +972,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,25 +983,25 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Milwaukee Brewers lefties (FD, DK)|Yelich, Shaw, Villar, |$9,400|37.6|4x|Success|</v>
+        <v>|Seattle Mariners hitters (FD, DK)|Segura, Heredia, Haniger, Healy|$11,800|25.2|2.14x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Colorado Rockies lefties (DK)|Blackmon, Dahl, Gonzalez, |$13,200|51|3.86x|Success|</v>
+        <v>|Atlanta Braves hitters (FD, DK)|Inciarte, Freeman, Markakis, Suzuki|$13,000|6|0.46x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Texas Rangers hitters (DK)|DeShields, Choo, Kiner-Falefa, Gallo|$14,700|34|2.31x|Success|</v>
+        <v>|Colorado Rockies righties (FD, DK)|Cuevas, Arenado, Story, Desmond|$16,500|46.9|2.84x|Failure|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+      <c r="A4" t="e">
         <f>CONCATENATE("|",Sheet1!A10,"|",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,", ",Sheet1!A15,"|",TEXT(Sheet1!B16,"$#,##0"),"|",Sheet1!C16,"|",CONCATENATE(ROUND(Sheet1!D16,2),"x"),"|",Sheet1!D17,"|")</f>
-        <v>|Chicago White Sox hitters (FD, DK)|Anderson, Abreu, Rondon, Palka|$12,600|36.9|2.93x|Failure|</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Latest players; revised cutoff for DK cheap hitters to $3500
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Current" sheetId="1" r:id="rId1"/>
+    <sheet name="RG table" sheetId="2" r:id="rId2"/>
+    <sheet name="Season Log" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Player</t>
   </si>
@@ -42,64 +43,104 @@
     <t>Total:</t>
   </si>
   <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
     <t>Failure</t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t>Colorado Rockies righties (FD, DK)</t>
-  </si>
-  <si>
-    <t>Desmond</t>
-  </si>
-  <si>
-    <t>Arenado</t>
-  </si>
-  <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Cuevas</t>
-  </si>
-  <si>
-    <t>Seattle Mariners hitters (FD, DK)</t>
-  </si>
-  <si>
-    <t>Atlanta Braves hitters (FD, DK)</t>
-  </si>
-  <si>
-    <t>Segura</t>
-  </si>
-  <si>
-    <t>Heredia</t>
-  </si>
-  <si>
-    <t>Haniger</t>
-  </si>
-  <si>
-    <t>Healy</t>
-  </si>
-  <si>
-    <t>Inciarte</t>
-  </si>
-  <si>
-    <t>Freeman</t>
-  </si>
-  <si>
-    <t>Markakis</t>
-  </si>
-  <si>
-    <t>Suzuki</t>
+    <t>Los Angeles Angels righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Boston Red Sox hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Detroit Tigers hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Chicago Cubs hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Blog Site</t>
+  </si>
+  <si>
+    <t>Draftshot</t>
+  </si>
+  <si>
+    <t>New York Yankees hitters (FD)</t>
+  </si>
+  <si>
+    <t>Toronto Blue Jays hitters (FD)</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Los Angeles Dodgers righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Houston Astros hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Toronto Blue Jays hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>McKinney</t>
+  </si>
+  <si>
+    <t>Drury</t>
+  </si>
+  <si>
+    <t>Smoak</t>
+  </si>
+  <si>
+    <t>Successes</t>
+  </si>
+  <si>
+    <t>Failures</t>
+  </si>
+  <si>
+    <t>Success Rate</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Bregman</t>
+  </si>
+  <si>
+    <t>Correa</t>
+  </si>
+  <si>
+    <t>Gurriel</t>
+  </si>
+  <si>
+    <t>Brantley</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -164,11 +205,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -188,10 +230,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -476,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,19 +541,19 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="F1" s="10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
@@ -551,51 +599,43 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5">
-        <v>3300</v>
+        <v>2200</v>
       </c>
       <c r="C3">
-        <v>15.7</v>
+        <v>3</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>4.7575757575757569</v>
+        <v>1.3636363636363638</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G3" s="5">
-        <v>2800</v>
+        <v>4200</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>24.2</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="5">
-        <v>3000</v>
-      </c>
-      <c r="M3">
-        <v>6.2</v>
-      </c>
-      <c r="N3" s="7">
+        <v>5.7619047619047619</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="N3" s="7" t="e">
         <f>(M3 / L3) * 1000</f>
-        <v>2.0666666666666669</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -605,112 +645,88 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G4" s="5">
-        <v>4300</v>
+        <v>3700</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>12.5</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="1">(H4 / G4) * 1000</f>
-        <v>1.3953488372093024</v>
-      </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="5">
-        <v>5400</v>
-      </c>
-      <c r="M4">
-        <v>28.7</v>
-      </c>
-      <c r="N4" s="7">
+        <v>3.3783783783783785</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="N4" s="7" t="e">
         <f t="shared" ref="N4:N7" si="2">(M4 / L4) * 1000</f>
-        <v>5.3148148148148149</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5">
-        <v>3500</v>
+        <v>2800</v>
       </c>
       <c r="C5">
-        <v>9.5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>2.7142857142857144</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G5" s="5">
-        <v>3400</v>
+        <v>3000</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="5">
-        <v>4400</v>
-      </c>
-      <c r="M5">
-        <v>6</v>
-      </c>
-      <c r="N5" s="7">
-        <f t="shared" si="2"/>
-        <v>1.3636363636363638</v>
+        <v>4.166666666666667</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="N5" s="7" t="e">
+        <f>(M5 / L5) * 1000</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
-        <v>2800</v>
+        <v>3600</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G6" s="5">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>6.2</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="5">
-        <v>3700</v>
-      </c>
-      <c r="M6">
-        <v>6</v>
-      </c>
-      <c r="N6" s="7">
-        <f t="shared" si="2"/>
-        <v>1.6216216216216215</v>
+        <v>2.2962962962962963</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="N6" s="7" t="e">
+        <f>(M6 / L6) * 1000</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -719,57 +735,55 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>11800</v>
+        <v>11100</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>25.2</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>2.1355932203389831</v>
+        <v>1.3513513513513513</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>13000</v>
+        <v>13600</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>6</v>
+        <v>55.400000000000006</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>0.46153846153846151</v>
+        <v>4.0735294117647056</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>16500</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>46.9</v>
-      </c>
-      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3" t="e">
         <f t="shared" si="2"/>
-        <v>2.8424242424242423</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>5</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="9"/>
@@ -950,7 +964,7 @@
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -982,41 +996,350 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>CONCATENATE("|",Sheet1!A1,"|",Sheet1!A3,", ",Sheet1!A4,", ",Sheet1!A5,", ",Sheet1!A6,"|",TEXT(Sheet1!B7,"$#,##0"),"|",Sheet1!C7,"|",CONCATENATE(ROUND(Sheet1!D7,2),"x"),"|",Sheet1!D8,"|")</f>
-        <v>|Seattle Mariners hitters (FD, DK)|Segura, Heredia, Haniger, Healy|$11,800|25.2|2.14x|Failure|</v>
+        <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
+        <v>|Toronto Blue Jays hitters (FD, DK)|Drury, McKinney, Hernandez, Smoak|$11,100|15|1.35x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>CONCATENATE("|",Sheet1!F1,"|",Sheet1!F3,", ",Sheet1!F4,", ",Sheet1!F5,", ",Sheet1!F6,"|",TEXT(Sheet1!G7,"$#,##0"),"|",Sheet1!H7,"|",CONCATENATE(ROUND(Sheet1!I7,2),"x"),"|",Sheet1!I8,"|")</f>
-        <v>|Atlanta Braves hitters (FD, DK)|Inciarte, Freeman, Markakis, Suzuki|$13,000|6|0.46x|Failure|</v>
+        <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
+        <v>|Houston Astros hitters (FD, DK)|Bregman, Brantley, Correa, Gurriel|$13,600|55.4|4.07x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>CONCATENATE("|",Sheet1!K1,"|",Sheet1!K3,", ",Sheet1!K4,", ",Sheet1!K5,", ",Sheet1!K6,"|",TEXT(Sheet1!L7,"$#,##0"),"|",Sheet1!M7,"|",CONCATENATE(ROUND(Sheet1!N7,2),"x"),"|",Sheet1!N8,"|")</f>
-        <v>|Colorado Rockies righties (FD, DK)|Cuevas, Arenado, Story, Desmond|$16,500|46.9|2.84x|Failure|</v>
+      <c r="A3" t="e">
+        <f>CONCATENATE("|",Current!K1,"|",Current!K3,", ",Current!K4,", ",Current!K5,", ",Current!K6,"|",TEXT(Current!L7,"$#,##0"),"|",Current!M7,"|",CONCATENATE(ROUND(Current!N7,2),"x"),"|",Current!N8,"|")</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="e">
-        <f>CONCATENATE("|",Sheet1!A10,"|",Sheet1!A12,", ",Sheet1!A13,", ",Sheet1!A14,", ",Sheet1!A15,"|",TEXT(Sheet1!B16,"$#,##0"),"|",Sheet1!C16,"|",CONCATENATE(ROUND(Sheet1!D16,2),"x"),"|",Sheet1!D17,"|")</f>
+        <f>CONCATENATE("|",Current!A10,"|",Current!A12,", ",Current!A13,", ",Current!A14,", ",Current!A15,"|",TEXT(Current!B16,"$#,##0"),"|",Current!C16,"|",CONCATENATE(ROUND(Current!D16,2),"x"),"|",Current!D17,"|")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="e">
-        <f>CONCATENATE("|",Sheet1!F10,"|",Sheet1!F12,", ",Sheet1!F13,", ",Sheet1!F14,", ",Sheet1!F15,"|",TEXT(Sheet1!G16,"$#,##0"),"|",Sheet1!H16,"|",CONCATENATE(ROUND(Sheet1!I16,2),"x"),"|",Sheet1!I17,"|")</f>
+        <f>CONCATENATE("|",Current!F10,"|",Current!F12,", ",Current!F13,", ",Current!F14,", ",Current!F15,"|",TEXT(Current!G16,"$#,##0"),"|",Current!H16,"|",CONCATENATE(ROUND(Current!I16,2),"x"),"|",Current!I17,"|")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="e">
-        <f>CONCATENATE("|",Sheet1!K10,"|",Sheet1!K12,", ",Sheet1!K13,", ",Sheet1!K14,", ",Sheet1!K15,"|",TEXT(Sheet1!L16,"$#,##0"),"|",Sheet1!M16,"|",CONCATENATE(ROUND(Sheet1!N16,2),"x"),"|",Sheet1!N17,"|")</f>
+        <f>CONCATENATE("|",Current!K10,"|",Current!K12,", ",Current!K13,", ",Current!K14,", ",Current!K15,"|",TEXT(Current!L16,"$#,##0"),"|",Current!M16,"|",CONCATENATE(ROUND(Current!N16,2),"x"),"|",Current!N17,"|")</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>43552</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>7.36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="14">
+        <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
+        <v>3</v>
+      </c>
+      <c r="I2" s="14">
+        <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
+        <v>2</v>
+      </c>
+      <c r="J2" s="15">
+        <f>H2 / (H2+I2)</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>43552</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>5.18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="14">
+        <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="14">
+        <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
+        <v>5</v>
+      </c>
+      <c r="J3" s="15">
+        <f>H3 / (H3+I3)</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>43552</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>43553</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>2.96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>43553</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>1.99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>43553</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>1.46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>43554</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>5.93</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>43554</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>43556</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>0.93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>43556</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>3.22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>43556</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>3.82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>43557</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>1.35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>43557</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>4.07</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added PA's/game per batting position & team runs scored
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="61">
   <si>
     <t>Player</t>
   </si>
@@ -160,34 +160,55 @@
     <t>Atlanta Braves hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Galvis</t>
+    <t>Hernandez</t>
   </si>
   <si>
     <t>Tampa Bay Rays hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Meadows</t>
-  </si>
-  <si>
-    <t>Pham</t>
-  </si>
-  <si>
-    <t>Choi</t>
-  </si>
-  <si>
-    <t>Lowe</t>
-  </si>
-  <si>
     <t>Toronto Blue Jays lefties (FD, DK)</t>
   </si>
   <si>
-    <t>Smoak</t>
-  </si>
-  <si>
-    <t>Tellez</t>
-  </si>
-  <si>
-    <t>Hanson</t>
+    <t>Boston Red Sox righties (FD)</t>
+  </si>
+  <si>
+    <t>Chicago White Sox hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>San Francisco Giants lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Baltimore Orioles hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Pittsburgh Pirates lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Moran</t>
+  </si>
+  <si>
+    <t>Pittsburgh Pirates hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Failure-XXX</t>
+  </si>
+  <si>
+    <t>Freese</t>
+  </si>
+  <si>
+    <t>Pollock</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Polanco</t>
+  </si>
+  <si>
+    <t>Kang</t>
+  </si>
+  <si>
+    <t>Diaz</t>
   </si>
 </sst>
 </file>
@@ -582,7 +603,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,13 +619,13 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="F1" s="15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -654,20 +675,26 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5">
-        <v>4200</v>
+        <v>3400</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="G3" s="5">
-        <v>3400</v>
+        <v>3500</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
@@ -681,24 +708,30 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5">
-        <v>3800</v>
+        <v>2400</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G4" s="5">
-        <v>3300</v>
+        <v>2600</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
       </c>
       <c r="I4" s="7">
         <f>(H4 / G4) * 1000</f>
-        <v>0</v>
+        <v>1.153846153846154</v>
       </c>
       <c r="L4" s="5"/>
       <c r="N4" s="7" t="e">
@@ -708,24 +741,30 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5">
-        <v>2700</v>
+        <v>3300</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>0</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G5" s="5">
-        <v>2600</v>
+        <v>2300</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
       </c>
       <c r="I5" s="7">
         <f>(H5 / G5) * 1000</f>
-        <v>0</v>
+        <v>1.3043478260869565</v>
       </c>
       <c r="L5" s="5"/>
       <c r="N5" s="7" t="e">
@@ -735,20 +774,26 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5">
-        <v>3600</v>
+        <v>2200</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
       <c r="D6" s="7">
         <f>(C6 / B6) * 1000</f>
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G6" s="5">
-        <v>2100</v>
+        <v>2000</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
       <c r="I6" s="7">
         <f>(H6 / G6) * 1000</f>
@@ -766,30 +811,30 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>14300</v>
+        <v>11300</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>0</v>
+        <v>0.26548672566371684</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>11400</v>
+        <v>10400</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I7" s="3">
         <f>(H7 / G7) * 1000</f>
-        <v>0</v>
+        <v>0.57692307692307698</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
@@ -808,8 +853,12 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1013,7 +1062,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,13 +1073,13 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|Tampa Bay Rays hitters (FD, DK)|Meadows, Pham, Choi, Lowe|$14,300|0|0x||</v>
+        <v>|Los Angeles Dodgers righties (FD, DK)|Hernandez, Freese, Pollock, Taylor|$11,300|3|0.27x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>|Toronto Blue Jays lefties (FD, DK)|Galvis, Smoak, Tellez, Hanson|$11,400|0|0x||</v>
+        <v>|Pittsburgh Pirates hitters (FD, DK)|Polanco, Moran, Kang, Diaz|$10,400|6|0.58x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1067,11 +1116,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,15 +1185,15 @@
       </c>
       <c r="H2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
-        <v>0.53846153846153844</v>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,15 +1217,15 @@
       </c>
       <c r="H3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.56666666666666665</v>
+        <v>0.47499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1886,6 +1935,12 @@
       <c r="C45" t="s">
         <v>45</v>
       </c>
+      <c r="D45">
+        <v>2.13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
@@ -1895,7 +1950,216 @@
         <v>19</v>
       </c>
       <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46">
+        <v>3.09</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>43572</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47">
+        <v>2.15</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>43572</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48">
+        <v>3.85</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>43573</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49">
+        <v>0.96</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>43573</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50">
+        <v>6.73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>43578</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51">
+        <v>1.95</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>43578</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>43578</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53">
+        <v>4.66</v>
+      </c>
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>43579</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
         <v>50</v>
+      </c>
+      <c r="D54">
+        <v>1.74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>43579</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55">
+        <v>0.91</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>43580</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56">
+        <v>0.27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>43580</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>43580</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>43580</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expanded to use games since season before last
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="71">
   <si>
     <t>Player</t>
   </si>
@@ -142,6 +142,9 @@
     <t>Pittsburgh Pirates righties (FD, DK)</t>
   </si>
   <si>
+    <t>Cabrera</t>
+  </si>
+  <si>
     <t>Arizona Diamondbacks lefties (FD, DK)</t>
   </si>
   <si>
@@ -160,7 +163,10 @@
     <t>Atlanta Braves hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Hernandez</t>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
   </si>
   <si>
     <t>Tampa Bay Rays hitters (FD, DK)</t>
@@ -184,31 +190,55 @@
     <t>Pittsburgh Pirates lefties (FD, DK)</t>
   </si>
   <si>
-    <t>Moran</t>
-  </si>
-  <si>
     <t>Pittsburgh Pirates hitters (FD, DK)</t>
   </si>
   <si>
     <t>Failure-XXX</t>
   </si>
   <si>
-    <t>Freese</t>
-  </si>
-  <si>
-    <t>Pollock</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Polanco</t>
-  </si>
-  <si>
-    <t>Kang</t>
-  </si>
-  <si>
-    <t>Diaz</t>
+    <t>Castellanos</t>
+  </si>
+  <si>
+    <t>Minnesota Twins hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>Washington Nationals righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Cincinnati Reds lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Milwaukee Brewers righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Cincinnati Reds hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Milwaukee Brewers hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>San Diego Padres hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Tampa Bay Rays righties (DK)</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Cleveland Indians righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Lindor</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Hicks</t>
   </si>
 </sst>
 </file>
@@ -603,7 +633,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,13 +649,13 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="F1" s="15" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -675,30 +705,30 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B3" s="5">
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>0</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="G3" s="5">
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>27.9</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>0</v>
+        <v>7.75</v>
       </c>
       <c r="L3" s="5"/>
       <c r="N3" s="7" t="e">
@@ -708,30 +738,30 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B4" s="5">
-        <v>2400</v>
+        <v>2700</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2900</v>
+      </c>
+      <c r="H4">
         <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2600</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
       </c>
       <c r="I4" s="7">
         <f>(H4 / G4) * 1000</f>
-        <v>1.153846153846154</v>
+        <v>0</v>
       </c>
       <c r="L4" s="5"/>
       <c r="N4" s="7" t="e">
@@ -741,30 +771,30 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5">
-        <v>3300</v>
+        <v>3100</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>21.7</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>0.90909090909090906</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G5" s="5">
-        <v>2300</v>
+        <v>3500</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I5" s="7">
         <f>(H5 / G5) * 1000</f>
-        <v>1.3043478260869565</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="L5" s="5"/>
       <c r="N5" s="7" t="e">
@@ -774,23 +804,23 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5">
-        <v>2200</v>
+        <v>2300</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" s="7">
         <f>(C6 / B6) * 1000</f>
-        <v>0</v>
+        <v>1.3043478260869565</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="5">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -811,30 +841,30 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>11300</v>
+        <v>11600</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>3</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>0.26548672566371684</v>
+        <v>2.9051724137931036</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>10400</v>
+        <v>12500</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>6</v>
+        <v>33.9</v>
       </c>
       <c r="I7" s="3">
         <f>(H7 / G7) * 1000</f>
-        <v>0.57692307692307698</v>
+        <v>2.7120000000000002</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
@@ -1073,13 +1103,13 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|Los Angeles Dodgers righties (FD, DK)|Hernandez, Freese, Pollock, Taylor|$11,300|3|0.27x|Failure|</v>
+        <v>|Detroit Tigers hitters (FD, DK)|Castellanos, Cabrera, Rodriguez, Hicks|$11,600|33.7|2.91x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>|Pittsburgh Pirates hitters (FD, DK)|Polanco, Moran, Kang, Diaz|$10,400|6|0.58x|Failure|</v>
+        <v>|Cleveland Indians hitters (FD, DK)|Lindor, Martin, Ramirez, Gonzalez|$12,500|33.9|2.71x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1116,11 +1146,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1215,7 @@
       </c>
       <c r="H2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
@@ -1193,7 +1223,7 @@
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
-        <v>0.53333333333333333</v>
+        <v>0.61111111111111116</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1217,15 +1247,15 @@
       </c>
       <c r="H3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.47499999999999998</v>
+        <v>0.47368421052631576</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1712,7 +1742,7 @@
         <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>6.96</v>
@@ -1746,7 +1776,7 @@
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34">
         <v>2.85</v>
@@ -1763,7 +1793,7 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D35">
         <v>4.83</v>
@@ -1780,7 +1810,7 @@
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D36">
         <v>9.85</v>
@@ -1814,7 +1844,7 @@
         <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D38">
         <v>0.22</v>
@@ -1831,7 +1861,7 @@
         <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D39">
         <v>5.54</v>
@@ -1899,7 +1929,7 @@
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D43">
         <v>5.73</v>
@@ -1933,7 +1963,7 @@
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D45">
         <v>2.13</v>
@@ -1950,7 +1980,7 @@
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D46">
         <v>3.09</v>
@@ -1967,7 +1997,7 @@
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D47">
         <v>2.15</v>
@@ -2052,7 +2082,7 @@
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D52">
         <v>1.1399999999999999</v>
@@ -2069,7 +2099,7 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D53">
         <v>4.66</v>
@@ -2086,7 +2116,7 @@
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D54">
         <v>1.74</v>
@@ -2103,7 +2133,7 @@
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D55">
         <v>0.91</v>
@@ -2137,13 +2167,13 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D57">
         <v>0.57999999999999996</v>
       </c>
       <c r="E57" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2153,6 +2183,15 @@
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58">
+        <v>4.54</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
@@ -2160,6 +2199,377 @@
       </c>
       <c r="B59" s="10" t="s">
         <v>16</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59">
+        <v>4.51</v>
+      </c>
+      <c r="E59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>43581</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" t="s">
+        <v>57</v>
+      </c>
+      <c r="D60">
+        <v>5.99</v>
+      </c>
+      <c r="E60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>43582</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s">
+        <v>57</v>
+      </c>
+      <c r="D61">
+        <v>8.31</v>
+      </c>
+      <c r="E61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>43582</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62">
+        <v>2.92</v>
+      </c>
+      <c r="E62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>43582</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63">
+        <v>2.81</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>43583</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64">
+        <v>4.51</v>
+      </c>
+      <c r="E64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
+        <v>43583</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>43583</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66">
+        <v>4.34</v>
+      </c>
+      <c r="E66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="11">
+        <v>43584</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" t="s">
+        <v>51</v>
+      </c>
+      <c r="D67">
+        <v>3.78</v>
+      </c>
+      <c r="E67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="11">
+        <v>43584</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>44</v>
+      </c>
+      <c r="D68">
+        <v>1.88</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="11">
+        <v>43585</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69">
+        <v>4.21</v>
+      </c>
+      <c r="E69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="11">
+        <v>43585</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="E70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="11">
+        <v>43586</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71">
+        <v>1.45</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="11">
+        <v>43586</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72">
+        <v>3.77</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="11">
+        <v>43586</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" t="s">
+        <v>64</v>
+      </c>
+      <c r="D73">
+        <v>2.06</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="11">
+        <v>43587</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="11">
+        <v>43587</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75">
+        <v>3.27</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="11">
+        <v>43587</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="11">
+        <v>43588</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="11">
+        <v>43588</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78">
+        <v>3.59</v>
+      </c>
+      <c r="E78" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="11">
+        <v>43589</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="11">
+        <v>43589</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80">
+        <v>2.91</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="11">
+        <v>43589</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81">
+        <v>2.71</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raised DK midrange & expensive hitter thresholds
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="80">
   <si>
     <t>Player</t>
   </si>
@@ -223,34 +223,49 @@
     <t>Washington Nationals hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Lindor</t>
-  </si>
-  <si>
-    <t>Kipnis</t>
-  </si>
-  <si>
-    <t>Ramirez</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
     <t>St. Louis Cardinals righties (FD, DK)</t>
   </si>
   <si>
     <t>Cleveland Indians lefties (FD, DK)</t>
   </si>
   <si>
-    <t>Dyson</t>
-  </si>
-  <si>
-    <t>Escobar</t>
-  </si>
-  <si>
-    <t>Peralta</t>
-  </si>
-  <si>
-    <t>Avila</t>
+    <t>New York Mets lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Texas Rangers hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>St Louis Cardinals hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Pederson</t>
+  </si>
+  <si>
+    <t>Muncy</t>
+  </si>
+  <si>
+    <t>Seager</t>
+  </si>
+  <si>
+    <t>Houston Astros righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Atlanta Braves righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>San Diego Padres righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Colorado Rockies lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>New York Mets hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Arizona Diamondbacks righties (FD, DK)</t>
   </si>
 </sst>
 </file>
@@ -645,7 +660,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,14 +676,12 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="F1" s="15" t="s">
-        <v>70</v>
-      </c>
+      <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
@@ -717,30 +730,22 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="5">
-        <v>2800</v>
+        <v>3700</v>
       </c>
       <c r="C3">
-        <v>24.4</v>
+        <v>28.2</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>8.7142857142857135</v>
-      </c>
-      <c r="F3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G3" s="5">
-        <v>3600</v>
-      </c>
-      <c r="H3">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="I3" s="7">
+        <v>7.6216216216216219</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="I3" s="7" t="e">
         <f>(H3 / G3) * 1000</f>
-        <v>9.5000000000000018</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L3" s="5"/>
       <c r="N3" s="7" t="e">
@@ -750,30 +755,22 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="5">
-        <v>3700</v>
+        <v>3400</v>
       </c>
       <c r="C4">
-        <v>37.9</v>
+        <v>6.2</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
-        <v>10.243243243243242</v>
-      </c>
-      <c r="F4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7">
+        <v>1.8235294117647058</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="I4" s="7" t="e">
         <f>(H4 / G4) * 1000</f>
-        <v>1.2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L4" s="5"/>
       <c r="N4" s="7" t="e">
@@ -783,30 +780,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5">
-        <v>4200</v>
+        <v>3000</v>
       </c>
       <c r="C5">
-        <v>22.2</v>
+        <v>27.6</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>5.2857142857142856</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="5">
-        <v>3500</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="I5" s="7" t="e">
         <f>(H5 / G5) * 1000</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L5" s="5"/>
       <c r="N5" s="7" t="e">
@@ -816,30 +805,22 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="5">
-        <v>2800</v>
+        <v>3100</v>
       </c>
       <c r="C6">
-        <v>21.7</v>
+        <v>28.4</v>
       </c>
       <c r="D6" s="7">
         <f>(C6 / B6) * 1000</f>
-        <v>7.75</v>
-      </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
+        <v>9.1612903225806459</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="I6" s="7" t="e">
         <f>(H6 / G6) * 1000</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L6" s="5"/>
       <c r="N6" s="7" t="e">
@@ -853,30 +834,30 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>13500</v>
+        <v>13200</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>106.2</v>
+        <v>90.4</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>7.866666666666668</v>
+        <v>6.8484848484848486</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>12100</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>37.200000000000003</v>
-      </c>
-      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="e">
         <f>(H7 / G7) * 1000</f>
-        <v>3.0743801652892566</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
@@ -898,9 +879,7 @@
       <c r="D8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="I8" s="8"/>
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1115,13 +1094,13 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|Arizona Diamondbacks lefties (FD, DK)|Dyson, Escobar, Peralta, Avila|$13,500|106.2|7.87x|Success|</v>
+        <v>|Los Angeles Dodgers hitters (FD, DK)|Pederson, Muncy, Turner, Seager|$13,200|90.4|6.85x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+      <c r="A2" t="e">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>|Cleveland Indians lefties (FD, DK)|Lindor, Kipnis, Ramirez, Gonzalez|$12,100|37.2|3.07x|Failure|</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1158,11 +1137,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <pane ySplit="3" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,15 +1206,15 @@
       </c>
       <c r="H2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1259,15 +1238,15 @@
       </c>
       <c r="H3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.51315789473684215</v>
+        <v>0.53921568627450978</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2855,6 +2834,15 @@
       <c r="B97" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="C97" t="s">
+        <v>53</v>
+      </c>
+      <c r="D97">
+        <v>8.08</v>
+      </c>
+      <c r="E97" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
@@ -2881,7 +2869,7 @@
         <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D99">
         <v>5.34</v>
@@ -2932,13 +2920,554 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D102">
         <v>3.07</v>
       </c>
       <c r="E102" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="11">
+        <v>43599</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103">
+        <v>5.72</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="11">
+        <v>43599</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C104" t="s">
+        <v>67</v>
+      </c>
+      <c r="D104">
+        <v>2.41</v>
+      </c>
+      <c r="E104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="11">
+        <v>43600</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C105" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105">
+        <v>1.5</v>
+      </c>
+      <c r="E105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="11">
+        <v>43600</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106" t="s">
+        <v>68</v>
+      </c>
+      <c r="D106">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E106" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="11">
+        <v>43601</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C107" t="s">
+        <v>67</v>
+      </c>
+      <c r="D107">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="E107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="11">
+        <v>43601</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108">
+        <v>0.98</v>
+      </c>
+      <c r="E108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="11">
+        <v>43601</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109">
+        <v>4.33</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="11">
+        <v>43602</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C110" t="s">
+        <v>69</v>
+      </c>
+      <c r="D110">
+        <v>1.74</v>
+      </c>
+      <c r="E110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="11">
+        <v>43602</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111">
+        <v>6.46</v>
+      </c>
+      <c r="E111" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="11">
+        <v>43603</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C112" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112">
+        <v>1.02</v>
+      </c>
+      <c r="E112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="11">
+        <v>43603</v>
+      </c>
+      <c r="B113" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" t="s">
+        <v>35</v>
+      </c>
+      <c r="D113">
+        <v>0.49</v>
+      </c>
+      <c r="E113" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="11">
+        <v>43603</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114" t="s">
+        <v>75</v>
+      </c>
+      <c r="D114">
+        <v>3.4</v>
+      </c>
+      <c r="E114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="11">
+        <v>43604</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" t="s">
+        <v>39</v>
+      </c>
+      <c r="D115">
+        <v>2.73</v>
+      </c>
+      <c r="E115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="11">
+        <v>43604</v>
+      </c>
+      <c r="B116" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" t="s">
+        <v>69</v>
+      </c>
+      <c r="D116">
+        <v>2.85</v>
+      </c>
+      <c r="E116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="11">
+        <v>43604</v>
+      </c>
+      <c r="B117" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" t="s">
+        <v>42</v>
+      </c>
+      <c r="D117">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="E117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="11">
+        <v>43605</v>
+      </c>
+      <c r="B118" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" t="s">
+        <v>73</v>
+      </c>
+      <c r="D118">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="11">
+        <v>43605</v>
+      </c>
+      <c r="B119" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C119" t="s">
+        <v>68</v>
+      </c>
+      <c r="D119">
+        <v>7.13</v>
+      </c>
+      <c r="E119" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="11">
+        <v>43605</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120" t="s">
+        <v>74</v>
+      </c>
+      <c r="D120">
+        <v>6.06</v>
+      </c>
+      <c r="E120" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="11">
+        <v>43606</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E121" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="11">
+        <v>43606</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122" t="s">
+        <v>53</v>
+      </c>
+      <c r="D122">
+        <v>6</v>
+      </c>
+      <c r="E122" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="11">
+        <v>43607</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C123" t="s">
+        <v>32</v>
+      </c>
+      <c r="D123">
+        <v>1.41</v>
+      </c>
+      <c r="E123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="11">
+        <v>43607</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C124" t="s">
+        <v>76</v>
+      </c>
+      <c r="D124">
+        <v>7.35</v>
+      </c>
+      <c r="E124" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="11">
+        <v>43607</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125" t="s">
+        <v>29</v>
+      </c>
+      <c r="D125">
+        <v>6.09</v>
+      </c>
+      <c r="E125" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="11">
+        <v>43607</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C126" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126">
+        <v>2.78</v>
+      </c>
+      <c r="E126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="11">
+        <v>43608</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" t="s">
+        <v>26</v>
+      </c>
+      <c r="D127">
+        <v>4.13</v>
+      </c>
+      <c r="E127" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="11">
+        <v>43608</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C128" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128">
+        <v>2.37</v>
+      </c>
+      <c r="E128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="11">
+        <v>43608</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C129" t="s">
+        <v>62</v>
+      </c>
+      <c r="E129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="11">
+        <v>43609</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C130" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130">
+        <v>7.29</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="11">
+        <v>43609</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C131" t="s">
+        <v>78</v>
+      </c>
+      <c r="D131">
+        <v>6.92</v>
+      </c>
+      <c r="E131" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="11">
+        <v>43610</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" t="s">
+        <v>79</v>
+      </c>
+      <c r="D132">
+        <v>7.67</v>
+      </c>
+      <c r="E132" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="11">
+        <v>43610</v>
+      </c>
+      <c r="B133" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" t="s">
+        <v>78</v>
+      </c>
+      <c r="D133">
+        <v>6.43</v>
+      </c>
+      <c r="E133" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="11">
+        <v>43611</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" t="s">
+        <v>63</v>
+      </c>
+      <c r="D134">
+        <v>6.85</v>
+      </c>
+      <c r="E134" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change pitcher FPTS/PA against switch hitters to be weighted avg of stats vs switch hitters and stats vs max(righties, lefties)
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="90">
   <si>
     <t>Player</t>
   </si>
@@ -238,13 +238,13 @@
     <t>St Louis Cardinals hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Pederson</t>
-  </si>
-  <si>
-    <t>Muncy</t>
-  </si>
-  <si>
-    <t>Seager</t>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>Goldschmidt</t>
+  </si>
+  <si>
+    <t>DeJong</t>
   </si>
   <si>
     <t>Houston Astros righties (FD, DK)</t>
@@ -259,13 +259,43 @@
     <t>Colorado Rockies lefties (FD, DK)</t>
   </si>
   <si>
-    <t>Turner</t>
-  </si>
-  <si>
     <t>New York Mets hitters (FD, DK)</t>
   </si>
   <si>
     <t>Arizona Diamondbacks righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Fowler</t>
+  </si>
+  <si>
+    <t>Pittsburgh Pirates hitters (FD)</t>
+  </si>
+  <si>
+    <t>Polanco</t>
+  </si>
+  <si>
+    <t>Marte</t>
+  </si>
+  <si>
+    <t>Moran</t>
+  </si>
+  <si>
+    <t>Tampa Bay Rays righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Pham</t>
+  </si>
+  <si>
+    <t>Adames</t>
+  </si>
+  <si>
+    <t>Robertson</t>
+  </si>
+  <si>
+    <t>Newman</t>
   </si>
 </sst>
 </file>
@@ -660,7 +690,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="K10" sqref="K10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,16 +706,20 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="F1" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="K1" s="15" t="s">
+        <v>80</v>
+      </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
@@ -730,27 +764,43 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5">
-        <v>3700</v>
+        <v>3000</v>
       </c>
       <c r="C3">
-        <v>28.2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>7.6216216216216219</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3400</v>
+      </c>
+      <c r="H3">
+        <v>24.9</v>
+      </c>
+      <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="N3" s="7" t="e">
+        <v>7.3235294117647056</v>
+      </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2400</v>
+      </c>
+      <c r="M3">
+        <v>29.2</v>
+      </c>
+      <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>12.166666666666666</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -758,74 +808,122 @@
         <v>71</v>
       </c>
       <c r="B4" s="5">
-        <v>3400</v>
+        <v>3700</v>
       </c>
       <c r="C4">
-        <v>6.2</v>
+        <v>21.7</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
-        <v>1.8235294117647058</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="I4" s="7" t="e">
+        <v>5.8648648648648649</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="5">
+        <v>3800</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4" s="7">
         <f>(H4 / G4) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="N4" s="7" t="e">
+        <v>1.5789473684210527</v>
+      </c>
+      <c r="K4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="5">
+        <v>3600</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
         <f>(M4 / L4) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B5" s="5">
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="C5">
-        <v>27.6</v>
+        <v>6.2</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="I5" s="7" t="e">
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2600</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="7">
         <f>(H5 / G5) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="N5" s="7" t="e">
+        <v>1.153846153846154</v>
+      </c>
+      <c r="K5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3500</v>
+      </c>
+      <c r="M5">
+        <v>9</v>
+      </c>
+      <c r="N5" s="7">
         <f>(M5 / L5) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>2.5714285714285712</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5">
-        <v>3100</v>
+        <v>3600</v>
       </c>
       <c r="C6">
-        <v>28.4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7">
         <f>(C6 / B6) * 1000</f>
-        <v>9.1612903225806459</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="I6" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2200</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6" s="7">
         <f>(H6 / G6) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="N6" s="7" t="e">
+        <v>2.7272727272727275</v>
+      </c>
+      <c r="K6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="5">
+        <v>2300</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
         <f>(M6 / L6) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -834,53 +932,57 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>13200</v>
+        <v>13900</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>90.4</v>
+        <v>27.9</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>6.8484848484848486</v>
+        <v>2.0071942446043165</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="e">
+        <v>39.9</v>
+      </c>
+      <c r="I7" s="3">
         <f>(H7 / G7) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>3.3249999999999997</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>0</v>
+        <v>11800</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="3" t="e">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="N7" s="3">
         <f>(M7 / L7) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>3.2372881355932206</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="N8" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="9"/>
@@ -1083,7 +1185,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,19 +1196,19 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|Los Angeles Dodgers hitters (FD, DK)|Pederson, Muncy, Turner, Seager|$13,200|90.4|6.85x|Success|</v>
+        <v>|St Louis Cardinals hitters (FD, DK)|Fowler, Goldschmidt, DeJong, Carpenter|$13,900|27.9|2.01x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
+      <c r="A2" t="str">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Tampa Bay Rays righties (FD, DK)|Garcia, Pham, Adames, Robertson|$12,000|39.9|3.33x|Failure|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="e">
+      <c r="A3" t="str">
         <f>CONCATENATE("|",Current!K1,"|",Current!K3,", ",Current!K4,", ",Current!K5,", ",Current!K6,"|",TEXT(Current!L7,"$#,##0"),"|",Current!M7,"|",CONCATENATE(ROUND(Current!N7,2),"x"),"|",Current!N8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Pittsburgh Pirates hitters (FD)|Newman, Polanco, Marte, Moran|$11,800|38.2|3.24x|Failure|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -1137,11 +1239,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
+      <pane ySplit="3" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E122" activeCellId="2" sqref="E130:E134 E124:E128 E119:E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,11 +1344,11 @@
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.53921568627450978</v>
+        <v>0.52380952380952384</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3410,7 +3512,7 @@
         <v>19</v>
       </c>
       <c r="C131" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D131">
         <v>6.92</v>
@@ -3427,7 +3529,7 @@
         <v>19</v>
       </c>
       <c r="C132" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D132">
         <v>7.67</v>
@@ -3444,7 +3546,7 @@
         <v>19</v>
       </c>
       <c r="C133" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D133">
         <v>6.43</v>
@@ -3468,6 +3570,74 @@
       </c>
       <c r="E134" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="11">
+        <v>43612</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C135" t="s">
+        <v>58</v>
+      </c>
+      <c r="D135">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="11">
+        <v>43613</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136" t="s">
+        <v>69</v>
+      </c>
+      <c r="D136">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="11">
+        <v>43613</v>
+      </c>
+      <c r="B137" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" t="s">
+        <v>84</v>
+      </c>
+      <c r="D137">
+        <v>3.33</v>
+      </c>
+      <c r="E137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="11">
+        <v>43613</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" t="s">
+        <v>80</v>
+      </c>
+      <c r="D138">
+        <v>3.24</v>
+      </c>
+      <c r="E138" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply ballpark factors to FPTS/PA given up by opposing pitchers
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="88">
   <si>
     <t>Player</t>
   </si>
@@ -238,15 +238,6 @@
     <t>St Louis Cardinals hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Carpenter</t>
-  </si>
-  <si>
-    <t>Goldschmidt</t>
-  </si>
-  <si>
-    <t>DeJong</t>
-  </si>
-  <si>
     <t>Houston Astros righties (FD, DK)</t>
   </si>
   <si>
@@ -265,37 +256,40 @@
     <t>Arizona Diamondbacks righties (FD, DK)</t>
   </si>
   <si>
-    <t>Fowler</t>
-  </si>
-  <si>
     <t>Pittsburgh Pirates hitters (FD)</t>
   </si>
   <si>
-    <t>Polanco</t>
-  </si>
-  <si>
-    <t>Marte</t>
-  </si>
-  <si>
-    <t>Moran</t>
-  </si>
-  <si>
     <t>Tampa Bay Rays righties (FD, DK)</t>
   </si>
   <si>
-    <t>Garcia</t>
-  </si>
-  <si>
-    <t>Pham</t>
-  </si>
-  <si>
-    <t>Adames</t>
-  </si>
-  <si>
-    <t>Robertson</t>
-  </si>
-  <si>
-    <t>Newman</t>
+    <t>Baltimore Orioles righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>Nunez</t>
+  </si>
+  <si>
+    <t>Broxton</t>
+  </si>
+  <si>
+    <t>Stewart</t>
+  </si>
+  <si>
+    <t>Arizona Diamondbacks hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Locastro</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Cron</t>
+  </si>
+  <si>
+    <t>Vargas</t>
   </si>
 </sst>
 </file>
@@ -690,7 +684,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:N10"/>
+      <selection activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,20 +700,18 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="F1" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
-      <c r="K1" s="15" t="s">
-        <v>80</v>
-      </c>
+      <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
@@ -767,163 +759,131 @@
         <v>79</v>
       </c>
       <c r="B3" s="5">
-        <v>3000</v>
+        <v>2700</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2500</v>
+      </c>
+      <c r="H3">
         <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="5">
-        <v>3400</v>
-      </c>
-      <c r="H3">
-        <v>24.9</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>7.3235294117647056</v>
-      </c>
-      <c r="K3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="5">
-        <v>2400</v>
-      </c>
-      <c r="M3">
-        <v>29.2</v>
-      </c>
-      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="N3" s="7" t="e">
         <f>(M3 / L3) * 1000</f>
-        <v>12.166666666666666</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B4" s="5">
-        <v>3700</v>
+        <v>3500</v>
       </c>
       <c r="C4">
-        <v>21.7</v>
+        <v>15.5</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
-        <v>5.8648648648648649</v>
+        <v>4.4285714285714288</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="5">
-        <v>3800</v>
+        <v>4000</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>18.7</v>
       </c>
       <c r="I4" s="7">
         <f>(H4 / G4) * 1000</f>
-        <v>1.5789473684210527</v>
-      </c>
-      <c r="K4" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="5">
-        <v>3600</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="7">
+        <v>4.6749999999999998</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="N4" s="7" t="e">
         <f>(M4 / L4) * 1000</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B5" s="5">
-        <v>3600</v>
+        <v>2300</v>
       </c>
       <c r="C5">
-        <v>6.2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>1.7222222222222223</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5" s="5">
-        <v>2600</v>
+        <v>2800</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>15.2</v>
       </c>
       <c r="I5" s="7">
         <f>(H5 / G5) * 1000</f>
-        <v>1.153846153846154</v>
-      </c>
-      <c r="K5" t="s">
-        <v>82</v>
-      </c>
-      <c r="L5" s="5">
-        <v>3500</v>
-      </c>
-      <c r="M5">
-        <v>9</v>
-      </c>
-      <c r="N5" s="7">
+        <v>5.4285714285714288</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="N5" s="7" t="e">
         <f>(M5 / L5) * 1000</f>
-        <v>2.5714285714285712</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5">
-        <v>3600</v>
+        <v>2300</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>18.7</v>
       </c>
       <c r="D6" s="7">
         <f>(C6 / B6) * 1000</f>
-        <v>0</v>
+        <v>8.1304347826086953</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="5">
-        <v>2200</v>
+        <v>3100</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I6" s="7">
         <f>(H6 / G6) * 1000</f>
-        <v>2.7272727272727275</v>
-      </c>
-      <c r="K6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" s="5">
-        <v>2300</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
+        <v>4.838709677419355</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="N6" s="7" t="e">
         <f>(M6 / L6) * 1000</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -932,45 +892,45 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>13900</v>
+        <v>10800</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>27.9</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>2.0071942446043165</v>
+        <v>3.4444444444444446</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>12000</v>
+        <v>12400</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>39.9</v>
+        <v>48.9</v>
       </c>
       <c r="I7" s="3">
         <f>(H7 / G7) * 1000</f>
-        <v>3.3249999999999997</v>
+        <v>3.9435483870967736</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>11800</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>38.200000000000003</v>
-      </c>
-      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3" t="e">
         <f>(M7 / L7) * 1000</f>
-        <v>3.2372881355932206</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -978,11 +938,9 @@
         <v>6</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="9"/>
@@ -1185,7 +1143,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,19 +1154,19 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|St Louis Cardinals hitters (FD, DK)|Fowler, Goldschmidt, DeJong, Carpenter|$13,900|27.9|2.01x|Failure|</v>
+        <v>|Baltimore Orioles hitters (FD, DK)|Alberto, Nunez, Stewart, Broxton|$10,800|37.2|3.44x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>|Tampa Bay Rays righties (FD, DK)|Garcia, Pham, Adames, Robertson|$12,000|39.9|3.33x|Failure|</v>
+        <v>|Arizona Diamondbacks hitters (FD, DK)|Locastro, Jones, Cron, Vargas|$12,400|48.9|3.94x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+      <c r="A3" t="e">
         <f>CONCATENATE("|",Current!K1,"|",Current!K3,", ",Current!K4,", ",Current!K5,", ",Current!K6,"|",TEXT(Current!L7,"$#,##0"),"|",Current!M7,"|",CONCATENATE(ROUND(Current!N7,2),"x"),"|",Current!N8,"|")</f>
-        <v>|Pittsburgh Pirates hitters (FD)|Newman, Polanco, Marte, Moran|$11,800|38.2|3.24x|Failure|</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -1239,11 +1197,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J138"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E122" activeCellId="2" sqref="E130:E134 E124:E128 E119:E122"/>
+      <pane ySplit="3" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1266,7 @@
       </c>
       <c r="H2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
@@ -1316,7 +1274,7 @@
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
-        <v>0.5</v>
+        <v>0.51851851851851849</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1340,15 +1298,15 @@
       </c>
       <c r="H3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.52380952380952384</v>
+        <v>0.52336448598130836</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3226,7 +3184,7 @@
         <v>16</v>
       </c>
       <c r="C114" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D114">
         <v>3.4</v>
@@ -3294,7 +3252,7 @@
         <v>19</v>
       </c>
       <c r="C118" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D118">
         <v>2.0099999999999998</v>
@@ -3328,7 +3286,7 @@
         <v>19</v>
       </c>
       <c r="C120" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D120">
         <v>6.06</v>
@@ -3396,7 +3354,7 @@
         <v>19</v>
       </c>
       <c r="C124" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D124">
         <v>7.35</v>
@@ -3512,7 +3470,7 @@
         <v>19</v>
       </c>
       <c r="C131" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D131">
         <v>6.92</v>
@@ -3529,7 +3487,7 @@
         <v>19</v>
       </c>
       <c r="C132" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D132">
         <v>7.67</v>
@@ -3546,7 +3504,7 @@
         <v>19</v>
       </c>
       <c r="C133" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D133">
         <v>6.43</v>
@@ -3557,16 +3515,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="11">
-        <v>43611</v>
+        <v>43610</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C134" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D134">
-        <v>6.85</v>
+        <v>5.39</v>
       </c>
       <c r="E134" t="s">
         <v>14</v>
@@ -3574,33 +3532,33 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="11">
-        <v>43612</v>
+        <v>43611</v>
       </c>
       <c r="B135" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C135" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D135">
-        <v>0.57999999999999996</v>
+        <v>6.85</v>
       </c>
       <c r="E135" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="11">
-        <v>43613</v>
+        <v>43612</v>
       </c>
       <c r="B136" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C136" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D136">
-        <v>2.0099999999999998</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E136" t="s">
         <v>6</v>
@@ -3614,10 +3572,10 @@
         <v>19</v>
       </c>
       <c r="C137" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D137">
-        <v>3.33</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="E137" t="s">
         <v>6</v>
@@ -3631,13 +3589,72 @@
         <v>19</v>
       </c>
       <c r="C138" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D138">
+        <v>3.33</v>
+      </c>
+      <c r="E138" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="11">
+        <v>43613</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C139" t="s">
+        <v>76</v>
+      </c>
+      <c r="D139">
         <v>3.24</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E139" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="11">
+        <v>43614</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C140" t="s">
+        <v>49</v>
+      </c>
+      <c r="D140">
+        <v>3.44</v>
+      </c>
+      <c r="E140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="11">
+        <v>43614</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141" t="s">
+        <v>83</v>
+      </c>
+      <c r="D141">
+        <v>3.94</v>
+      </c>
+      <c r="E141" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="11">
+        <v>43615</v>
+      </c>
+      <c r="B142" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted stack value score to emphasize value over total FPTS
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="98">
   <si>
     <t>Player</t>
   </si>
@@ -271,25 +271,55 @@
     <t>Nunez</t>
   </si>
   <si>
+    <t>Severino</t>
+  </si>
+  <si>
     <t>Broxton</t>
   </si>
   <si>
-    <t>Stewart</t>
-  </si>
-  <si>
     <t>Arizona Diamondbacks hitters (FD, DK)</t>
   </si>
   <si>
-    <t>Locastro</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Cron</t>
-  </si>
-  <si>
-    <t>Vargas</t>
+    <t>Colorado Rockies hitters (FD, DK)</t>
+  </si>
+  <si>
+    <t>Colorado Rockies hitters (DK)</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Adames</t>
+  </si>
+  <si>
+    <t>Zunino</t>
+  </si>
+  <si>
+    <t>Choo</t>
+  </si>
+  <si>
+    <t>DeShields</t>
+  </si>
+  <si>
+    <t>Cabrera</t>
+  </si>
+  <si>
+    <t>Odor</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Eaton</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Dozier (INJ)</t>
   </si>
 </sst>
 </file>
@@ -684,7 +714,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,18 +730,20 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="F1" s="15" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="K1" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
@@ -756,134 +788,166 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5">
-        <v>2700</v>
+        <v>3400</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>6.2</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>1.1111111111111112</v>
+        <v>1.8235294117647058</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G3" s="5">
         <v>2500</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="N3" s="7" t="e">
+        <v>7.3599999999999994</v>
+      </c>
+      <c r="K3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="5">
+        <v>3900</v>
+      </c>
+      <c r="M3">
+        <v>31.4</v>
+      </c>
+      <c r="N3" s="7">
         <f>(M3 / L3) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>8.0512820512820511</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B4" s="5">
         <v>3500</v>
       </c>
       <c r="C4">
-        <v>15.5</v>
+        <v>22.2</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
-        <v>4.4285714285714288</v>
+        <v>6.3428571428571425</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G4" s="5">
-        <v>4000</v>
+        <v>3600</v>
       </c>
       <c r="H4">
-        <v>18.7</v>
+        <v>6.2</v>
       </c>
       <c r="I4" s="7">
         <f>(H4 / G4) * 1000</f>
-        <v>4.6749999999999998</v>
-      </c>
-      <c r="L4" s="5"/>
-      <c r="N4" s="7" t="e">
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="K4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="5">
+        <v>2400</v>
+      </c>
+      <c r="M4">
+        <v>18.2</v>
+      </c>
+      <c r="N4" s="7">
         <f>(M4 / L4) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>7.583333333333333</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B5" s="5">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>0</v>
+        <v>12.88</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G5" s="5">
         <v>2800</v>
       </c>
       <c r="H5">
-        <v>15.2</v>
+        <v>59.6</v>
       </c>
       <c r="I5" s="7">
         <f>(H5 / G5) * 1000</f>
-        <v>5.4285714285714288</v>
-      </c>
-      <c r="L5" s="5"/>
-      <c r="N5" s="7" t="e">
+        <v>21.285714285714285</v>
+      </c>
+      <c r="K5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3200</v>
+      </c>
+      <c r="M5">
+        <v>22.2</v>
+      </c>
+      <c r="N5" s="7">
         <f>(M5 / L5) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>6.9375</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B6" s="5">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="C6">
-        <v>18.7</v>
+        <v>0</v>
       </c>
       <c r="D6" s="7">
         <f>(C6 / B6) * 1000</f>
-        <v>8.1304347826086953</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G6" s="5">
-        <v>3100</v>
+        <v>2400</v>
       </c>
       <c r="H6">
-        <v>15</v>
+        <v>30.9</v>
       </c>
       <c r="I6" s="7">
         <f>(H6 / G6) * 1000</f>
-        <v>4.838709677419355</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="N6" s="7" t="e">
+        <v>12.875</v>
+      </c>
+      <c r="K6" t="s">
+        <v>93</v>
+      </c>
+      <c r="L6" s="5">
+        <v>2600</v>
+      </c>
+      <c r="M6">
+        <v>12.9</v>
+      </c>
+      <c r="N6" s="7">
         <f>(M6 / L6) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>4.9615384615384617</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -892,55 +956,57 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>10800</v>
+        <v>11900</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>37.200000000000003</v>
+        <v>60.6</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>3.4444444444444446</v>
+        <v>5.0924369747899156</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>12400</v>
+        <v>11300</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>48.9</v>
+        <v>115.1</v>
       </c>
       <c r="I7" s="3">
         <f>(H7 / G7) * 1000</f>
-        <v>3.9435483870967736</v>
+        <v>10.185840707964601</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="L7" s="6">
         <f>SUM(L3:L6)</f>
-        <v>0</v>
+        <v>12100</v>
       </c>
       <c r="M7" s="1">
         <f>SUM(M3:M6)</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="3" t="e">
+        <v>84.7</v>
+      </c>
+      <c r="N7" s="3">
         <f>(M7 / L7) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="8"/>
+      <c r="N8" s="8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="9"/>
@@ -948,7 +1014,9 @@
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -1000,10 +1068,18 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="D12" s="7" t="e">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3800</v>
+      </c>
+      <c r="C12">
+        <v>15.4</v>
+      </c>
+      <c r="D12" s="7">
         <f>(C12 / B12) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>4.0526315789473681</v>
       </c>
       <c r="G12" s="5"/>
       <c r="I12" s="7" t="e">
@@ -1017,10 +1093,18 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="D13" s="7" t="e">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3100</v>
+      </c>
+      <c r="C13">
+        <v>15.4</v>
+      </c>
+      <c r="D13" s="7">
         <f>(C13 / B13) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>4.967741935483871</v>
       </c>
       <c r="G13" s="5"/>
       <c r="I13" s="7" t="e">
@@ -1034,10 +1118,18 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="D14" s="7" t="e">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C14">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D14" s="7">
         <f>(C14 / B14) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>3.0666666666666664</v>
       </c>
       <c r="G14" s="5"/>
       <c r="I14" s="7" t="e">
@@ -1051,10 +1143,18 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="D15" s="7" t="e">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2800</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7">
         <f>(C15 / B15) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>1.0714285714285714</v>
       </c>
       <c r="G15" s="5"/>
       <c r="I15" s="7" t="e">
@@ -1073,15 +1173,15 @@
       </c>
       <c r="B16" s="6">
         <f>SUM(B12:B15)</f>
-        <v>0</v>
+        <v>12700</v>
       </c>
       <c r="C16" s="1">
         <f>SUM(C12:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="e">
+        <v>43</v>
+      </c>
+      <c r="D16" s="3">
         <f>(C16 / B16) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>3.3858267716535435</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>4</v>
@@ -1115,7 +1215,9 @@
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="8"/>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="N17" s="8"/>
     </row>
@@ -1143,7 +1245,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,25 +1256,25 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|Baltimore Orioles hitters (FD, DK)|Alberto, Nunez, Stewart, Broxton|$10,800|37.2|3.44x|Failure|</v>
+        <v>|Tampa Bay Rays hitters (FD, DK)|Diaz, Garcia, Adames, Zunino|$11,900|60.6|5.09x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>|Arizona Diamondbacks hitters (FD, DK)|Locastro, Jones, Cron, Vargas|$12,400|48.9|3.94x|Success|</v>
+        <v>|Baltimore Orioles hitters (FD, DK)|Alberto, Nunez, Severino, Broxton|$11,300|115.1|10.19x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="e">
+      <c r="A3" t="str">
         <f>CONCATENATE("|",Current!K1,"|",Current!K3,", ",Current!K4,", ",Current!K5,", ",Current!K6,"|",TEXT(Current!L7,"$#,##0"),"|",Current!M7,"|",CONCATENATE(ROUND(Current!N7,2),"x"),"|",Current!N8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Texas Rangers hitters (FD, DK)|Choo, DeShields, Cabrera, Odor|$12,100|84.7|7x|Success|</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="e">
+      <c r="A4" t="str">
         <f>CONCATENATE("|",Current!A10,"|",Current!A12,", ",Current!A13,", ",Current!A14,", ",Current!A15,"|",TEXT(Current!B16,"$#,##0"),"|",Current!C16,"|",CONCATENATE(ROUND(Current!D16,2),"x"),"|",Current!D17,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Washington Nationals hitters (FD, DK)|Turner, Eaton, Adams, Dozier (INJ)|$12,700|43|3.39x|Failure|</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1197,11 +1299,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C142" sqref="C142"/>
+      <pane ySplit="3" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,11 +1372,11 @@
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
-        <v>0.51851851851851849</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1298,15 +1400,15 @@
       </c>
       <c r="H3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.52336448598130836</v>
+        <v>0.52542372881355937</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3655,6 +3757,210 @@
       </c>
       <c r="B142" s="10" t="s">
         <v>16</v>
+      </c>
+      <c r="C142" t="s">
+        <v>42</v>
+      </c>
+      <c r="D142">
+        <v>3.34</v>
+      </c>
+      <c r="E142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="11">
+        <v>43616</v>
+      </c>
+      <c r="B143" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" t="s">
+        <v>42</v>
+      </c>
+      <c r="D143">
+        <v>3.07</v>
+      </c>
+      <c r="E143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="11">
+        <v>43616</v>
+      </c>
+      <c r="B144" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C144" t="s">
+        <v>26</v>
+      </c>
+      <c r="D144">
+        <v>0.46</v>
+      </c>
+      <c r="E144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="11">
+        <v>43616</v>
+      </c>
+      <c r="B145" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" t="s">
+        <v>27</v>
+      </c>
+      <c r="D145">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="11">
+        <v>43616</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C146" t="s">
+        <v>84</v>
+      </c>
+      <c r="D146">
+        <v>9.08</v>
+      </c>
+      <c r="E146" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="11">
+        <v>43617</v>
+      </c>
+      <c r="B147" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="11">
+        <v>43618</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C148" t="s">
+        <v>85</v>
+      </c>
+      <c r="D148">
+        <v>2.46</v>
+      </c>
+      <c r="E148" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="11">
+        <v>43618</v>
+      </c>
+      <c r="B149" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C149" t="s">
+        <v>49</v>
+      </c>
+      <c r="D149">
+        <v>0.27</v>
+      </c>
+      <c r="E149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="11">
+        <v>43619</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C150" t="s">
+        <v>21</v>
+      </c>
+      <c r="D150">
+        <v>3.74</v>
+      </c>
+      <c r="E150" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="11">
+        <v>43620</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C151" t="s">
+        <v>44</v>
+      </c>
+      <c r="D151">
+        <v>5.09</v>
+      </c>
+      <c r="E151" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="11">
+        <v>43620</v>
+      </c>
+      <c r="B152" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C152" t="s">
+        <v>49</v>
+      </c>
+      <c r="D152">
+        <v>10.19</v>
+      </c>
+      <c r="E152" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="11">
+        <v>43620</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C153" t="s">
+        <v>68</v>
+      </c>
+      <c r="D153">
+        <v>7</v>
+      </c>
+      <c r="E153" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="11">
+        <v>43620</v>
+      </c>
+      <c r="B154" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C154" t="s">
+        <v>64</v>
+      </c>
+      <c r="D154">
+        <v>3.39</v>
+      </c>
+      <c r="E154" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
When looking up MLB player ID by display name, ignore " Jr"
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="94">
   <si>
     <t>Player</t>
   </si>
@@ -284,6 +284,30 @@
   </si>
   <si>
     <t>Minnesota Twins righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Tampa Bay Rays lefties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Betts</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Vazquez</t>
+  </si>
+  <si>
+    <t>St Louis Cardinals righties (FD, DK)</t>
+  </si>
+  <si>
+    <t>Edman</t>
+  </si>
+  <si>
+    <t>Goldschmidt</t>
+  </si>
+  <si>
+    <t>O'Neill</t>
   </si>
 </sst>
 </file>
@@ -677,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,12 +718,14 @@
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="F1" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
@@ -747,15 +773,31 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="D3" s="7" t="e">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4300</v>
+      </c>
+      <c r="C3">
+        <v>25.1</v>
+      </c>
+      <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="7" t="e">
+        <v>5.837209302325582</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2800</v>
+      </c>
+      <c r="H3">
+        <v>15.5</v>
+      </c>
+      <c r="I3" s="7">
         <f>(H3 / G3) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>5.5357142857142856</v>
       </c>
       <c r="L3" s="5"/>
       <c r="N3" s="7" t="e">
@@ -764,15 +806,31 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="D4" s="7" t="e">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4400</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="I4" s="7" t="e">
+        <v>0.68181818181818188</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2700</v>
+      </c>
+      <c r="H4">
+        <v>18.7</v>
+      </c>
+      <c r="I4" s="7">
         <f>(H4 / G4) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>6.9259259259259256</v>
       </c>
       <c r="L4" s="5"/>
       <c r="N4" s="7" t="e">
@@ -781,15 +839,31 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="D5" s="7" t="e">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C5">
+        <v>12.2</v>
+      </c>
+      <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="I5" s="7" t="e">
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3100</v>
+      </c>
+      <c r="H5">
+        <v>28.2</v>
+      </c>
+      <c r="I5" s="7">
         <f>(H5 / G5) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>9.0967741935483879</v>
       </c>
       <c r="L5" s="5"/>
       <c r="N5" s="7" t="e">
@@ -803,10 +877,18 @@
         <f>(C6 / B6) * 1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="I6" s="7" t="e">
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2300</v>
+      </c>
+      <c r="H6">
+        <v>12.2</v>
+      </c>
+      <c r="I6" s="7">
         <f>(H6 / G6) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>5.3043478260869561</v>
       </c>
       <c r="L6" s="5"/>
       <c r="N6" s="7" t="e">
@@ -820,30 +902,30 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>0</v>
+        <v>11700</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="e">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>3.4444444444444442</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(G3:G6)</f>
-        <v>0</v>
+        <v>10900</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(H3:H6)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="e">
+        <v>74.600000000000009</v>
+      </c>
+      <c r="I7" s="3">
         <f>(H7 / G7) * 1000</f>
-        <v>#DIV/0!</v>
+        <v>6.8440366972477067</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>4</v>
@@ -862,8 +944,12 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1066,7 +1152,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1074,15 +1162,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="e">
+      <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|Boston Red Sox hitters (FD, DK)|Betts, Martinez, Vazquez, |$11,700|40.3|3.44x|Failure|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
+      <c r="A2" t="str">
         <f>CONCATENATE("|",Current!F1,"|",Current!F3,", ",Current!F4,", ",Current!F5,", ",Current!F6,"|",TEXT(Current!G7,"$#,##0"),"|",Current!H7,"|",CONCATENATE(ROUND(Current!I7,2),"x"),"|",Current!I8,"|")</f>
-        <v>#DIV/0!</v>
+        <v>|St Louis Cardinals righties (FD, DK)|Edman, Martinez, Goldschmidt, O'Neill|$10,900|74.6|6.84x|Success|</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1119,11 +1207,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J200"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F200" sqref="F200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F209" sqref="F209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,11 +1276,11 @@
       </c>
       <c r="H2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
@@ -1220,15 +1308,15 @@
       </c>
       <c r="H3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Success")</f>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I3" s="13">
         <f>COUNTIFS(B:B,"RG",E:E,"Failure")</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="J3" s="14">
         <f>H3 / (H3+I3)</f>
-        <v>0.55128205128205132</v>
+        <v>0.53658536585365857</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -4530,6 +4618,15 @@
       <c r="B198" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="C198" t="s">
+        <v>58</v>
+      </c>
+      <c r="D198">
+        <v>4.37</v>
+      </c>
+      <c r="E198" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="11">
@@ -4563,6 +4660,159 @@
       </c>
       <c r="E200" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="11">
+        <v>43648</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C201" t="s">
+        <v>86</v>
+      </c>
+      <c r="D201">
+        <v>3.02</v>
+      </c>
+      <c r="E201" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="11">
+        <v>43648</v>
+      </c>
+      <c r="B202" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C202" t="s">
+        <v>80</v>
+      </c>
+      <c r="D202">
+        <v>3.22</v>
+      </c>
+      <c r="E202" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="11">
+        <v>43648</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C203" t="s">
+        <v>63</v>
+      </c>
+      <c r="D203">
+        <v>2.09</v>
+      </c>
+      <c r="E203" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="11">
+        <v>43649</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C204" t="s">
+        <v>55</v>
+      </c>
+      <c r="D204">
+        <v>1.27</v>
+      </c>
+      <c r="E204" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="11">
+        <v>43649</v>
+      </c>
+      <c r="B205" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C205" t="s">
+        <v>40</v>
+      </c>
+      <c r="D205">
+        <v>0.84</v>
+      </c>
+      <c r="E205" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="11">
+        <v>43649</v>
+      </c>
+      <c r="B206" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C206" t="s">
+        <v>27</v>
+      </c>
+      <c r="D206">
+        <v>5.16</v>
+      </c>
+      <c r="E206" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="11">
+        <v>43650</v>
+      </c>
+      <c r="B207" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C207" t="s">
+        <v>35</v>
+      </c>
+      <c r="D207">
+        <v>3.6</v>
+      </c>
+      <c r="E207" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="11">
+        <v>43651</v>
+      </c>
+      <c r="B208" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C208" t="s">
+        <v>8</v>
+      </c>
+      <c r="D208">
+        <v>3.44</v>
+      </c>
+      <c r="E208" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="11">
+        <v>43651</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C209" t="s">
+        <v>90</v>
+      </c>
+      <c r="D209">
+        <v>6.84</v>
+      </c>
+      <c r="E209" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prep for 2020 season
</commit_message>
<xml_diff>
--- a/dfs-tools/build/Blog_stack_value_results.xlsx
+++ b/dfs-tools/build/Blog_stack_value_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="112">
   <si>
     <t>Player</t>
   </si>
@@ -305,18 +305,6 @@
     <t>San Francisco Giants righties (FD, DK)</t>
   </si>
   <si>
-    <t>Villar</t>
-  </si>
-  <si>
-    <t>Mancini</t>
-  </si>
-  <si>
-    <t>Santander</t>
-  </si>
-  <si>
-    <t>Nunez</t>
-  </si>
-  <si>
     <t>Min Value</t>
   </si>
   <si>
@@ -369,6 +357,15 @@
   </si>
   <si>
     <t>Blog Site:</t>
+  </si>
+  <si>
+    <t>Bichette</t>
+  </si>
+  <si>
+    <t>Galvis</t>
+  </si>
+  <si>
+    <t>Guerrero</t>
   </si>
 </sst>
 </file>
@@ -470,14 +467,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -733,11 +730,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="41"/>
-        <c:axId val="242736480"/>
-        <c:axId val="242742752"/>
+        <c:axId val="32704968"/>
+        <c:axId val="32706144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="242736480"/>
+        <c:axId val="32704968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242742752"/>
+        <c:crossAx val="32706144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -839,7 +836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242742752"/>
+        <c:axId val="32706144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +910,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242736480"/>
+        <c:crossAx val="32704968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1884,7 +1881,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,20 +1896,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="A1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1954,17 +1951,17 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="B3" s="5">
-        <v>3000</v>
+        <v>3300</v>
       </c>
       <c r="C3">
-        <v>3.5</v>
+        <v>12.2</v>
       </c>
       <c r="D3" s="7">
         <f>(C3 / B3) * 1000</f>
-        <v>1.1666666666666667</v>
+        <v>3.6969696969696968</v>
       </c>
       <c r="G3" s="5"/>
       <c r="I3" s="7" t="e">
@@ -1979,17 +1976,17 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B4" s="5">
-        <v>3800</v>
+        <v>2800</v>
       </c>
       <c r="C4">
-        <v>18.7</v>
+        <v>24.7</v>
       </c>
       <c r="D4" s="7">
         <f>(C4 / B4) * 1000</f>
-        <v>4.9210526315789478</v>
+        <v>8.8214285714285712</v>
       </c>
       <c r="G4" s="5"/>
       <c r="I4" s="7" t="e">
@@ -2004,17 +2001,17 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B5" s="5">
-        <v>3400</v>
+        <v>3600</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="D5" s="7">
         <f>(C5 / B5) * 1000</f>
-        <v>0</v>
+        <v>4.3055555555555554</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="7" t="e">
@@ -2028,18 +2025,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="5">
-        <v>3400</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="5"/>
+      <c r="D6" s="7" t="e">
         <f>(C6 / B6) * 1000</f>
-        <v>0.88235294117647067</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G6" s="5"/>
       <c r="I6" s="7" t="e">
@@ -2058,15 +2047,15 @@
       </c>
       <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
-        <v>13600</v>
+        <v>9700</v>
       </c>
       <c r="C7" s="1">
         <f>SUM(C3:C6)</f>
-        <v>25.2</v>
+        <v>52.4</v>
       </c>
       <c r="D7" s="3">
         <f>(C7 / B7) * 1000</f>
-        <v>1.8529411764705883</v>
+        <v>5.4020618556701034</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -2101,7 +2090,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I8" s="8"/>
       <c r="N8" s="8"/>
@@ -2112,18 +2101,18 @@
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2316,7 +2305,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("|",Current!A1,"|",Current!A3,", ",Current!A4,", ",Current!A5,", ",Current!A6,"|",TEXT(Current!B7,"$#,##0"),"|",Current!C7,"|",CONCATENATE(ROUND(Current!D7,2),"x"),"|",Current!D8,"|")</f>
-        <v>|Baltimore Orioles hitters (FD, DK)|Villar, Mancini, Santander, Nunez|$13,600|25.2|1.85x|Failure|</v>
+        <v>|Toronto Blue Jays hitters (FD, DK)|Bichette, Galvis, Guerrero, |$9,700|52.4|5.4x|Success|</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2359,11 +2348,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J246"/>
+  <dimension ref="A1:J247"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F247" sqref="F247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,7 +2417,7 @@
       </c>
       <c r="H2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Success")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="13">
         <f>COUNTIFS(B:B,"Draftshot",E:E,"Failure")</f>
@@ -2436,7 +2425,7 @@
       </c>
       <c r="J2" s="14">
         <f>H2 / (H2+I2)</f>
-        <v>0.51111111111111107</v>
+        <v>0.52173913043478259</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6594,6 +6583,23 @@
       </c>
       <c r="E246" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="11">
+        <v>43680</v>
+      </c>
+      <c r="B247" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C247" t="s">
+        <v>22</v>
+      </c>
+      <c r="D247">
+        <v>5.4</v>
+      </c>
+      <c r="E247" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -6607,7 +6613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -6622,24 +6628,24 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6651,21 +6657,21 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D2">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A2,'Season Log (2019)'!D:D,"&lt;"&amp;B2,'Season Log (2019)'!B:B,I$1)</f>
         <v>12</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <f>D2/I$2</f>
         <v>6.0606060606060608E-2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="17">
+      <c r="I2" s="16">
         <f>SUM(D:D)</f>
         <v>198</v>
       </c>
@@ -6678,13 +6684,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A3,'Season Log (2019)'!D:D,"&lt;"&amp;B3,'Season Log (2019)'!B:B,I$1)</f>
         <v>27</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <f t="shared" ref="E3:E12" si="0">D3/I$2</f>
         <v>0.13636363636363635</v>
       </c>
@@ -6697,13 +6703,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D4">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A4,'Season Log (2019)'!D:D,"&lt;"&amp;B4,'Season Log (2019)'!B:B,I$1)</f>
         <v>32</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <f t="shared" si="0"/>
         <v>0.16161616161616163</v>
       </c>
@@ -6716,13 +6722,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A5,'Season Log (2019)'!D:D,"&lt;"&amp;B5,'Season Log (2019)'!B:B,I$1)</f>
         <v>35</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <f t="shared" si="0"/>
         <v>0.17676767676767677</v>
       </c>
@@ -6735,13 +6741,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D6">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A6,'Season Log (2019)'!D:D,"&lt;"&amp;B6,'Season Log (2019)'!B:B,I$1)</f>
         <v>37</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <f t="shared" si="0"/>
         <v>0.18686868686868688</v>
       </c>
@@ -6754,13 +6760,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D7">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A7,'Season Log (2019)'!D:D,"&lt;"&amp;B7,'Season Log (2019)'!B:B,I$1)</f>
         <v>17</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f t="shared" si="0"/>
         <v>8.5858585858585856E-2</v>
       </c>
@@ -6773,13 +6779,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D8">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A8,'Season Log (2019)'!D:D,"&lt;"&amp;B8,'Season Log (2019)'!B:B,I$1)</f>
         <v>16</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f t="shared" si="0"/>
         <v>8.0808080808080815E-2</v>
       </c>
@@ -6792,13 +6798,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D9">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A9,'Season Log (2019)'!D:D,"&lt;"&amp;B9,'Season Log (2019)'!B:B,I$1)</f>
         <v>11</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
@@ -6811,13 +6817,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A10,'Season Log (2019)'!D:D,"&lt;"&amp;B10,'Season Log (2019)'!B:B,I$1)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <f t="shared" si="0"/>
         <v>2.0202020202020204E-2</v>
       </c>
@@ -6830,13 +6836,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D11">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A11,'Season Log (2019)'!D:D,"&lt;"&amp;B11,'Season Log (2019)'!B:B,I$1)</f>
         <v>5</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <f t="shared" si="0"/>
         <v>2.5252525252525252E-2</v>
       </c>
@@ -6849,13 +6855,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <f>COUNTIFS('Season Log (2019)'!D:D,"&gt;="&amp;A12,'Season Log (2019)'!D:D,"&lt;"&amp;B12,'Season Log (2019)'!B:B,I$1)</f>
         <v>2</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <f t="shared" si="0"/>
         <v>1.0101010101010102E-2</v>
       </c>

</xml_diff>